<commit_message>
bug fixes, RTF writing out properly with new enhancements. Formatting improvements in table 14-2.01
</commit_message>
<xml_diff>
--- a/scripts/table_examples/titles.xlsx
+++ b/scripts/table_examples/titles.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16105\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A507E77-58F4-4E72-AA88-CC96B2EDB310}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CC76DE-AFD6-4461-83F7-6EE7590FF1D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{45CA4081-01D7-4010-B007-0BB33FDF9BEF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{45CA4081-01D7-4010-B007-0BB33FDF9BEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$225</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -834,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278D11AC-8C4C-4475-BF03-113D4886E6A9}">
   <dimension ref="A1:I225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
-      <selection activeCell="B229" sqref="B229"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,7 +1000,7 @@
         <v>1</v>
       </c>
       <c r="G6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" t="b">
         <v>1</v>
@@ -1023,7 +1027,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" t="b">
         <v>1</v>
@@ -1146,7 +1150,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" t="b">
         <v>1</v>
@@ -1170,7 +1174,7 @@
         <v>1</v>
       </c>
       <c r="G13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" t="b">
         <v>1</v>
@@ -1197,7 +1201,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" t="b">
         <v>1</v>
@@ -1320,7 +1324,7 @@
         <v>1</v>
       </c>
       <c r="G19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" t="b">
         <v>1</v>
@@ -1344,7 +1348,7 @@
         <v>1</v>
       </c>
       <c r="G20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" t="b">
         <v>1</v>
@@ -1371,7 +1375,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" t="b">
         <v>1</v>
@@ -1494,7 +1498,7 @@
         <v>1</v>
       </c>
       <c r="G26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26" t="b">
         <v>1</v>
@@ -1518,7 +1522,7 @@
         <v>1</v>
       </c>
       <c r="G27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" t="b">
         <v>1</v>
@@ -1545,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" t="b">
         <v>1</v>
@@ -1668,7 +1672,7 @@
         <v>1</v>
       </c>
       <c r="G33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33" t="b">
         <v>1</v>
@@ -1692,7 +1696,7 @@
         <v>1</v>
       </c>
       <c r="G34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34" t="b">
         <v>1</v>
@@ -1716,7 +1720,7 @@
         <v>1</v>
       </c>
       <c r="G35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" t="b">
         <v>1</v>
@@ -1743,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36" t="b">
         <v>1</v>
@@ -1866,7 +1870,7 @@
         <v>1</v>
       </c>
       <c r="G41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41" t="b">
         <v>1</v>
@@ -1890,7 +1894,7 @@
         <v>1</v>
       </c>
       <c r="G42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42" t="b">
         <v>1</v>
@@ -1914,7 +1918,7 @@
         <v>1</v>
       </c>
       <c r="G43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" t="b">
         <v>1</v>
@@ -1941,7 +1945,7 @@
         <v>0</v>
       </c>
       <c r="G44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H44" t="b">
         <v>1</v>
@@ -2064,7 +2068,7 @@
         <v>1</v>
       </c>
       <c r="G49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H49" t="b">
         <v>1</v>
@@ -2088,7 +2092,7 @@
         <v>1</v>
       </c>
       <c r="G50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H50" t="b">
         <v>1</v>
@@ -2112,7 +2116,7 @@
         <v>1</v>
       </c>
       <c r="G51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H51" t="b">
         <v>1</v>
@@ -2139,7 +2143,7 @@
         <v>0</v>
       </c>
       <c r="G52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H52" t="b">
         <v>1</v>
@@ -2262,7 +2266,7 @@
         <v>1</v>
       </c>
       <c r="G57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H57" t="b">
         <v>1</v>
@@ -2286,7 +2290,7 @@
         <v>1</v>
       </c>
       <c r="G58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H58" t="b">
         <v>1</v>
@@ -2310,7 +2314,7 @@
         <v>1</v>
       </c>
       <c r="G59" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H59" t="b">
         <v>1</v>
@@ -2337,7 +2341,7 @@
         <v>0</v>
       </c>
       <c r="G60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H60" t="b">
         <v>1</v>
@@ -2460,7 +2464,7 @@
         <v>1</v>
       </c>
       <c r="G65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H65" t="b">
         <v>1</v>
@@ -2484,7 +2488,7 @@
         <v>1</v>
       </c>
       <c r="G66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H66" t="b">
         <v>1</v>
@@ -2508,7 +2512,7 @@
         <v>1</v>
       </c>
       <c r="G67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67" t="b">
         <v>1</v>
@@ -2535,7 +2539,7 @@
         <v>0</v>
       </c>
       <c r="G68" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H68" t="b">
         <v>1</v>
@@ -2658,7 +2662,7 @@
         <v>1</v>
       </c>
       <c r="G73" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H73" t="b">
         <v>1</v>
@@ -2682,7 +2686,7 @@
         <v>1</v>
       </c>
       <c r="G74" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H74" t="b">
         <v>1</v>
@@ -2706,7 +2710,7 @@
         <v>1</v>
       </c>
       <c r="G75" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H75" t="b">
         <v>1</v>
@@ -2733,7 +2737,7 @@
         <v>0</v>
       </c>
       <c r="G76" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H76" t="b">
         <v>1</v>
@@ -2856,7 +2860,7 @@
         <v>1</v>
       </c>
       <c r="G81" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H81" t="b">
         <v>1</v>
@@ -2880,7 +2884,7 @@
         <v>1</v>
       </c>
       <c r="G82" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H82" t="b">
         <v>1</v>
@@ -2904,7 +2908,7 @@
         <v>1</v>
       </c>
       <c r="G83" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H83" t="b">
         <v>1</v>
@@ -2928,7 +2932,7 @@
         <v>1</v>
       </c>
       <c r="G84" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H84" t="b">
         <v>1</v>
@@ -2955,7 +2959,7 @@
         <v>0</v>
       </c>
       <c r="G85" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H85" t="b">
         <v>1</v>
@@ -3066,7 +3070,7 @@
         <v>44</v>
       </c>
       <c r="G90" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H90" t="b">
         <v>1</v>
@@ -3087,7 +3091,7 @@
         <v>49</v>
       </c>
       <c r="G91" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H91" t="b">
         <v>1</v>
@@ -3108,7 +3112,7 @@
         <v>50</v>
       </c>
       <c r="G92" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H92" t="b">
         <v>1</v>
@@ -3135,7 +3139,7 @@
         <v>0</v>
       </c>
       <c r="G93" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H93" t="b">
         <v>1</v>
@@ -3258,7 +3262,7 @@
         <v>1</v>
       </c>
       <c r="G98" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H98" t="b">
         <v>1</v>
@@ -3282,7 +3286,7 @@
         <v>1</v>
       </c>
       <c r="G99" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H99" t="b">
         <v>1</v>
@@ -3306,7 +3310,7 @@
         <v>1</v>
       </c>
       <c r="G100" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H100" t="b">
         <v>1</v>
@@ -3333,7 +3337,7 @@
         <v>0</v>
       </c>
       <c r="G101" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H101" t="b">
         <v>1</v>
@@ -3459,7 +3463,7 @@
         <v>0</v>
       </c>
       <c r="G106" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H106" t="b">
         <v>1</v>
@@ -3579,7 +3583,7 @@
         <v>80</v>
       </c>
       <c r="G111" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H111" t="b">
         <v>1</v>
@@ -3606,7 +3610,7 @@
         <v>0</v>
       </c>
       <c r="G112" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H112" t="b">
         <v>1</v>
@@ -3729,7 +3733,7 @@
         <v>1</v>
       </c>
       <c r="G117" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H117" t="b">
         <v>1</v>
@@ -3753,7 +3757,7 @@
         <v>1</v>
       </c>
       <c r="G118" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H118" t="b">
         <v>1</v>
@@ -3777,7 +3781,7 @@
         <v>1</v>
       </c>
       <c r="G119" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H119" t="b">
         <v>1</v>
@@ -3804,7 +3808,7 @@
         <v>0</v>
       </c>
       <c r="G120" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H120" t="b">
         <v>1</v>
@@ -3927,7 +3931,7 @@
         <v>1</v>
       </c>
       <c r="G125" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H125" t="b">
         <v>1</v>
@@ -3954,7 +3958,7 @@
         <v>0</v>
       </c>
       <c r="G126" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H126" t="b">
         <v>1</v>
@@ -4077,7 +4081,7 @@
         <v>1</v>
       </c>
       <c r="G131" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H131" t="b">
         <v>1</v>
@@ -4101,7 +4105,7 @@
         <v>1</v>
       </c>
       <c r="G132" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H132" t="b">
         <v>1</v>
@@ -4128,7 +4132,7 @@
         <v>0</v>
       </c>
       <c r="G133" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H133" t="b">
         <v>1</v>
@@ -4251,7 +4255,7 @@
         <v>1</v>
       </c>
       <c r="G138" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H138" t="b">
         <v>1</v>
@@ -4275,7 +4279,7 @@
         <v>1</v>
       </c>
       <c r="G139" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H139" t="b">
         <v>1</v>
@@ -4299,7 +4303,7 @@
         <v>1</v>
       </c>
       <c r="G140" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H140" t="b">
         <v>1</v>
@@ -4323,7 +4327,7 @@
         <v>1</v>
       </c>
       <c r="G141" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H141" t="b">
         <v>1</v>
@@ -4347,7 +4351,7 @@
         <v>1</v>
       </c>
       <c r="G142" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H142" t="b">
         <v>1</v>
@@ -4374,7 +4378,7 @@
         <v>0</v>
       </c>
       <c r="G143" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H143" t="b">
         <v>1</v>
@@ -4497,7 +4501,7 @@
         <v>1</v>
       </c>
       <c r="G148" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H148" t="b">
         <v>1</v>
@@ -4521,7 +4525,7 @@
         <v>1</v>
       </c>
       <c r="G149" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H149" t="b">
         <v>1</v>
@@ -4545,7 +4549,7 @@
         <v>1</v>
       </c>
       <c r="G150" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H150" t="b">
         <v>1</v>
@@ -4569,7 +4573,7 @@
         <v>1</v>
       </c>
       <c r="G151" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H151" t="b">
         <v>1</v>
@@ -4593,7 +4597,7 @@
         <v>1</v>
       </c>
       <c r="G152" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H152" t="b">
         <v>1</v>
@@ -4620,7 +4624,7 @@
         <v>0</v>
       </c>
       <c r="G153" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H153" t="b">
         <v>1</v>
@@ -4743,7 +4747,7 @@
         <v>1</v>
       </c>
       <c r="G158" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H158" t="b">
         <v>1</v>
@@ -4770,7 +4774,7 @@
         <v>0</v>
       </c>
       <c r="G159" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H159" t="b">
         <v>1</v>
@@ -4893,7 +4897,7 @@
         <v>1</v>
       </c>
       <c r="G164" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H164" t="b">
         <v>1</v>
@@ -4920,7 +4924,7 @@
         <v>0</v>
       </c>
       <c r="G165" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H165" t="b">
         <v>1</v>
@@ -5043,7 +5047,7 @@
         <v>1</v>
       </c>
       <c r="G170" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H170" t="b">
         <v>1</v>
@@ -5070,7 +5074,7 @@
         <v>0</v>
       </c>
       <c r="G171" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H171" t="b">
         <v>1</v>
@@ -5193,7 +5197,7 @@
         <v>1</v>
       </c>
       <c r="G176" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H176" t="b">
         <v>1</v>
@@ -5217,7 +5221,7 @@
         <v>1</v>
       </c>
       <c r="G177" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H177" t="b">
         <v>1</v>
@@ -5244,7 +5248,7 @@
         <v>0</v>
       </c>
       <c r="G178" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H178" t="b">
         <v>1</v>
@@ -5367,7 +5371,7 @@
         <v>1</v>
       </c>
       <c r="G183" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H183" t="b">
         <v>1</v>
@@ -5391,7 +5395,7 @@
         <v>1</v>
       </c>
       <c r="G184" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H184" t="b">
         <v>1</v>
@@ -5415,7 +5419,7 @@
         <v>1</v>
       </c>
       <c r="G185" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H185" t="b">
         <v>1</v>
@@ -5439,7 +5443,7 @@
         <v>1</v>
       </c>
       <c r="G186" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H186" t="b">
         <v>1</v>
@@ -5466,7 +5470,7 @@
         <v>0</v>
       </c>
       <c r="G187" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H187" t="b">
         <v>1</v>
@@ -5589,7 +5593,7 @@
         <v>1</v>
       </c>
       <c r="G192" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H192" t="b">
         <v>1</v>
@@ -5613,7 +5617,7 @@
         <v>1</v>
       </c>
       <c r="G193" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H193" t="b">
         <v>1</v>
@@ -5637,7 +5641,7 @@
         <v>1</v>
       </c>
       <c r="G194" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H194" t="b">
         <v>1</v>
@@ -5661,7 +5665,7 @@
         <v>1</v>
       </c>
       <c r="G195" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H195" t="b">
         <v>1</v>
@@ -5688,7 +5692,7 @@
         <v>0</v>
       </c>
       <c r="G196" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H196" t="b">
         <v>1</v>
@@ -5811,7 +5815,7 @@
         <v>1</v>
       </c>
       <c r="G201" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H201" t="b">
         <v>1</v>
@@ -5838,7 +5842,7 @@
         <v>0</v>
       </c>
       <c r="G202" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H202" t="b">
         <v>1</v>
@@ -5961,7 +5965,7 @@
         <v>1</v>
       </c>
       <c r="G207" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H207" t="b">
         <v>1</v>
@@ -5988,7 +5992,7 @@
         <v>0</v>
       </c>
       <c r="G208" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H208" t="b">
         <v>1</v>
@@ -6111,7 +6115,7 @@
         <v>1</v>
       </c>
       <c r="G213" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H213" t="b">
         <v>1</v>
@@ -6138,7 +6142,7 @@
         <v>0</v>
       </c>
       <c r="G214" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H214" t="b">
         <v>1</v>
@@ -6264,7 +6268,7 @@
         <v>0</v>
       </c>
       <c r="G219" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H219" t="b">
         <v>1</v>
@@ -6387,7 +6391,7 @@
         <v>1</v>
       </c>
       <c r="G224" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H224" t="b">
         <v>1</v>
@@ -6414,13 +6418,14 @@
         <v>0</v>
       </c>
       <c r="G225" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H225" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I225" xr:uid="{D7EA4A85-694E-4AFC-88A1-1F9A25E65D09}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Table 14-3.01 - 14-3.09 done, with repeating tables took out both portions of the table into funcs.R. Fixed titles as well.
</commit_message>
<xml_diff>
--- a/scripts/table_examples/titles.xlsx
+++ b/scripts/table_examples/titles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16105\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CC76DE-AFD6-4461-83F7-6EE7590FF1D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89460901-7272-434E-8B62-C146B3A73170}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{45CA4081-01D7-4010-B007-0BB33FDF9BEF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{45CA4081-01D7-4010-B007-0BB33FDF9BEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$225</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="149">
   <si>
     <t>split</t>
   </si>
@@ -99,9 +98,6 @@
     <t>DATE_FORMAT: %H:%M %A, %B %d, %Y</t>
   </si>
   <si>
-    <t>FILE_PATH: Source %s</t>
-  </si>
-  <si>
     <t>14-1.01</t>
   </si>
   <si>
@@ -484,6 +480,9 @@
   </si>
   <si>
     <t>index</t>
+  </si>
+  <si>
+    <t>FILE_PATH: Source: %s</t>
   </si>
 </sst>
 </file>
@@ -838,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278D11AC-8C4C-4475-BF03-113D4886E6A9}">
   <dimension ref="A1:I225"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
+      <selection activeCell="F224" sqref="F224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,7 +858,7 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
@@ -885,7 +884,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2">
         <f>IF(AND(A1=A2, C1=C2), B1+1, 1)</f>
@@ -912,7 +911,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B66" si="0">IF(AND(A2=A3, C2=C3), B2+1, 1)</f>
@@ -936,7 +935,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
@@ -960,7 +959,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
@@ -984,7 +983,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
@@ -1008,7 +1007,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
@@ -1018,7 +1017,7 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
@@ -1035,7 +1034,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <f>IF(AND(A7=A8, C7=C8), B7+1, 1)</f>
@@ -1062,7 +1061,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
@@ -1072,7 +1071,7 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" t="s">
         <v>1</v>
@@ -1086,7 +1085,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
@@ -1096,7 +1095,7 @@
         <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" t="s">
         <v>2</v>
@@ -1110,7 +1109,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
@@ -1120,7 +1119,7 @@
         <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11" t="s">
         <v>2</v>
@@ -1134,7 +1133,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
@@ -1144,7 +1143,7 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" t="s">
         <v>1</v>
@@ -1158,7 +1157,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
@@ -1168,7 +1167,7 @@
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13" t="s">
         <v>1</v>
@@ -1182,7 +1181,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
@@ -1192,7 +1191,7 @@
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E14" t="s">
         <v>19</v>
@@ -1209,7 +1208,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
@@ -1236,7 +1235,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
@@ -1260,7 +1259,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
@@ -1270,7 +1269,7 @@
         <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F17" t="s">
         <v>2</v>
@@ -1284,7 +1283,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
@@ -1294,7 +1293,7 @@
         <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F18" t="s">
         <v>2</v>
@@ -1308,7 +1307,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
@@ -1318,7 +1317,7 @@
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F19" t="s">
         <v>1</v>
@@ -1332,7 +1331,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
@@ -1342,7 +1341,7 @@
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F20" t="s">
         <v>1</v>
@@ -1356,7 +1355,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
@@ -1366,7 +1365,7 @@
         <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E21" t="s">
         <v>19</v>
@@ -1383,7 +1382,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
@@ -1410,7 +1409,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
@@ -1420,7 +1419,7 @@
         <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F23" t="s">
         <v>1</v>
@@ -1434,7 +1433,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
@@ -1444,7 +1443,7 @@
         <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F24" t="s">
         <v>2</v>
@@ -1458,7 +1457,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
@@ -1468,7 +1467,7 @@
         <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F25" t="s">
         <v>2</v>
@@ -1482,7 +1481,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
@@ -1492,7 +1491,7 @@
         <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F26" t="s">
         <v>1</v>
@@ -1506,7 +1505,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
@@ -1516,7 +1515,7 @@
         <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F27" t="s">
         <v>1</v>
@@ -1530,7 +1529,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
@@ -1540,7 +1539,7 @@
         <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E28" t="s">
         <v>19</v>
@@ -1557,7 +1556,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
@@ -1584,7 +1583,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
@@ -1594,7 +1593,7 @@
         <v>13</v>
       </c>
       <c r="D30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F30" t="s">
         <v>1</v>
@@ -1608,7 +1607,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
@@ -1618,7 +1617,7 @@
         <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F31" t="s">
         <v>2</v>
@@ -1632,7 +1631,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
@@ -1642,7 +1641,7 @@
         <v>13</v>
       </c>
       <c r="D32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F32" t="s">
         <v>2</v>
@@ -1656,7 +1655,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33">
         <f t="shared" si="0"/>
@@ -1666,7 +1665,7 @@
         <v>18</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F33" t="s">
         <v>1</v>
@@ -1680,7 +1679,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
@@ -1690,7 +1689,7 @@
         <v>18</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F34" t="s">
         <v>1</v>
@@ -1704,7 +1703,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
@@ -1714,7 +1713,7 @@
         <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F35" t="s">
         <v>1</v>
@@ -1728,7 +1727,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
@@ -1738,7 +1737,7 @@
         <v>18</v>
       </c>
       <c r="D36" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E36" t="s">
         <v>19</v>
@@ -1755,7 +1754,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
@@ -1782,7 +1781,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
@@ -1792,7 +1791,7 @@
         <v>13</v>
       </c>
       <c r="D38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F38" t="s">
         <v>1</v>
@@ -1806,7 +1805,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
@@ -1816,7 +1815,7 @@
         <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F39" t="s">
         <v>2</v>
@@ -1830,7 +1829,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40">
         <f t="shared" si="0"/>
@@ -1840,7 +1839,7 @@
         <v>13</v>
       </c>
       <c r="D40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F40" t="s">
         <v>2</v>
@@ -1854,7 +1853,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
@@ -1864,7 +1863,7 @@
         <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F41" t="s">
         <v>1</v>
@@ -1878,7 +1877,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B42">
         <f t="shared" si="0"/>
@@ -1888,7 +1887,7 @@
         <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F42" t="s">
         <v>1</v>
@@ -1902,7 +1901,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B43">
         <f t="shared" si="0"/>
@@ -1912,7 +1911,7 @@
         <v>18</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F43" t="s">
         <v>1</v>
@@ -1926,7 +1925,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44">
         <f t="shared" si="0"/>
@@ -1936,7 +1935,7 @@
         <v>18</v>
       </c>
       <c r="D44" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E44" t="s">
         <v>19</v>
@@ -1953,7 +1952,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B45">
         <f t="shared" si="0"/>
@@ -1980,7 +1979,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46">
         <f t="shared" si="0"/>
@@ -1990,7 +1989,7 @@
         <v>13</v>
       </c>
       <c r="D46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F46" t="s">
         <v>1</v>
@@ -2004,7 +2003,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B47">
         <f t="shared" si="0"/>
@@ -2014,7 +2013,7 @@
         <v>13</v>
       </c>
       <c r="D47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F47" t="s">
         <v>2</v>
@@ -2028,7 +2027,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B48">
         <f t="shared" si="0"/>
@@ -2038,7 +2037,7 @@
         <v>13</v>
       </c>
       <c r="D48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F48" t="s">
         <v>2</v>
@@ -2052,7 +2051,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B49">
         <f t="shared" si="0"/>
@@ -2062,7 +2061,7 @@
         <v>18</v>
       </c>
       <c r="D49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F49" t="s">
         <v>1</v>
@@ -2076,7 +2075,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B50">
         <f t="shared" si="0"/>
@@ -2086,7 +2085,7 @@
         <v>18</v>
       </c>
       <c r="D50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F50" t="s">
         <v>1</v>
@@ -2100,7 +2099,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51">
         <f t="shared" si="0"/>
@@ -2110,7 +2109,7 @@
         <v>18</v>
       </c>
       <c r="D51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F51" t="s">
         <v>1</v>
@@ -2124,7 +2123,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52">
         <f t="shared" si="0"/>
@@ -2134,7 +2133,7 @@
         <v>18</v>
       </c>
       <c r="D52" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E52" t="s">
         <v>19</v>
@@ -2151,7 +2150,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B53">
         <f t="shared" si="0"/>
@@ -2178,7 +2177,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54">
         <f t="shared" si="0"/>
@@ -2188,7 +2187,7 @@
         <v>13</v>
       </c>
       <c r="D54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F54" t="s">
         <v>1</v>
@@ -2202,7 +2201,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55">
         <f t="shared" si="0"/>
@@ -2212,7 +2211,7 @@
         <v>13</v>
       </c>
       <c r="D55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F55" t="s">
         <v>2</v>
@@ -2226,7 +2225,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56">
         <f t="shared" si="0"/>
@@ -2236,7 +2235,7 @@
         <v>13</v>
       </c>
       <c r="D56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F56" t="s">
         <v>2</v>
@@ -2250,7 +2249,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B57">
         <f t="shared" si="0"/>
@@ -2260,7 +2259,7 @@
         <v>18</v>
       </c>
       <c r="D57" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F57" t="s">
         <v>1</v>
@@ -2274,7 +2273,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B58">
         <f t="shared" si="0"/>
@@ -2284,7 +2283,7 @@
         <v>18</v>
       </c>
       <c r="D58" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F58" t="s">
         <v>1</v>
@@ -2298,7 +2297,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B59">
         <f t="shared" si="0"/>
@@ -2308,7 +2307,7 @@
         <v>18</v>
       </c>
       <c r="D59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F59" t="s">
         <v>1</v>
@@ -2322,7 +2321,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B60">
         <f t="shared" si="0"/>
@@ -2332,7 +2331,7 @@
         <v>18</v>
       </c>
       <c r="D60" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E60" t="s">
         <v>19</v>
@@ -2349,7 +2348,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B61">
         <f t="shared" si="0"/>
@@ -2376,7 +2375,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B62">
         <f t="shared" si="0"/>
@@ -2386,7 +2385,7 @@
         <v>13</v>
       </c>
       <c r="D62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F62" t="s">
         <v>1</v>
@@ -2400,7 +2399,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B63">
         <f t="shared" si="0"/>
@@ -2410,7 +2409,7 @@
         <v>13</v>
       </c>
       <c r="D63" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F63" t="s">
         <v>2</v>
@@ -2424,7 +2423,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B64">
         <f t="shared" si="0"/>
@@ -2434,7 +2433,7 @@
         <v>13</v>
       </c>
       <c r="D64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F64" t="s">
         <v>2</v>
@@ -2448,7 +2447,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B65">
         <f t="shared" si="0"/>
@@ -2458,7 +2457,7 @@
         <v>18</v>
       </c>
       <c r="D65" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F65" t="s">
         <v>1</v>
@@ -2472,7 +2471,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B66">
         <f t="shared" si="0"/>
@@ -2482,7 +2481,7 @@
         <v>18</v>
       </c>
       <c r="D66" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F66" t="s">
         <v>1</v>
@@ -2496,7 +2495,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B67">
         <f t="shared" ref="B67:B130" si="1">IF(AND(A66=A67, C66=C67), B66+1, 1)</f>
@@ -2506,7 +2505,7 @@
         <v>18</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F67" t="s">
         <v>1</v>
@@ -2520,7 +2519,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B68">
         <f t="shared" si="1"/>
@@ -2530,7 +2529,7 @@
         <v>18</v>
       </c>
       <c r="D68" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E68" t="s">
         <v>19</v>
@@ -2547,7 +2546,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B69">
         <f t="shared" si="1"/>
@@ -2574,7 +2573,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B70">
         <f t="shared" si="1"/>
@@ -2584,7 +2583,7 @@
         <v>13</v>
       </c>
       <c r="D70" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F70" t="s">
         <v>1</v>
@@ -2598,7 +2597,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B71">
         <f t="shared" si="1"/>
@@ -2608,7 +2607,7 @@
         <v>13</v>
       </c>
       <c r="D71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F71" t="s">
         <v>2</v>
@@ -2622,7 +2621,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B72">
         <f t="shared" si="1"/>
@@ -2632,7 +2631,7 @@
         <v>13</v>
       </c>
       <c r="D72" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F72" t="s">
         <v>2</v>
@@ -2646,7 +2645,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B73">
         <f t="shared" si="1"/>
@@ -2656,7 +2655,7 @@
         <v>18</v>
       </c>
       <c r="D73" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F73" t="s">
         <v>1</v>
@@ -2670,7 +2669,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B74">
         <f t="shared" si="1"/>
@@ -2680,7 +2679,7 @@
         <v>18</v>
       </c>
       <c r="D74" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F74" t="s">
         <v>1</v>
@@ -2694,7 +2693,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B75">
         <f t="shared" si="1"/>
@@ -2704,7 +2703,7 @@
         <v>18</v>
       </c>
       <c r="D75" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F75" t="s">
         <v>1</v>
@@ -2718,7 +2717,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B76">
         <f t="shared" si="1"/>
@@ -2728,7 +2727,7 @@
         <v>18</v>
       </c>
       <c r="D76" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E76" t="s">
         <v>19</v>
@@ -2745,7 +2744,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B77">
         <f t="shared" si="1"/>
@@ -2772,7 +2771,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B78">
         <f t="shared" si="1"/>
@@ -2782,7 +2781,7 @@
         <v>13</v>
       </c>
       <c r="D78" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F78" t="s">
         <v>1</v>
@@ -2796,7 +2795,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B79">
         <f t="shared" si="1"/>
@@ -2806,7 +2805,7 @@
         <v>13</v>
       </c>
       <c r="D79" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F79" t="s">
         <v>2</v>
@@ -2820,7 +2819,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B80">
         <f t="shared" si="1"/>
@@ -2830,7 +2829,7 @@
         <v>13</v>
       </c>
       <c r="D80" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F80" t="s">
         <v>2</v>
@@ -2844,7 +2843,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B81">
         <f t="shared" si="1"/>
@@ -2854,7 +2853,7 @@
         <v>18</v>
       </c>
       <c r="D81" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F81" t="s">
         <v>1</v>
@@ -2868,7 +2867,7 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B82">
         <f t="shared" si="1"/>
@@ -2878,7 +2877,7 @@
         <v>18</v>
       </c>
       <c r="D82" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F82" t="s">
         <v>1</v>
@@ -2892,7 +2891,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B83">
         <f t="shared" si="1"/>
@@ -2902,7 +2901,7 @@
         <v>18</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F83" t="s">
         <v>1</v>
@@ -2916,7 +2915,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B84">
         <f t="shared" si="1"/>
@@ -2926,7 +2925,7 @@
         <v>18</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F84" t="s">
         <v>1</v>
@@ -2940,7 +2939,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B85">
         <f t="shared" si="1"/>
@@ -2950,7 +2949,7 @@
         <v>18</v>
       </c>
       <c r="D85" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E85" t="s">
         <v>19</v>
@@ -2967,7 +2966,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B86">
         <f t="shared" si="1"/>
@@ -2994,7 +2993,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B87">
         <f t="shared" si="1"/>
@@ -3004,7 +3003,10 @@
         <v>13</v>
       </c>
       <c r="D87" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="F87" t="s">
+        <v>1</v>
       </c>
       <c r="G87" t="b">
         <v>1</v>
@@ -3015,7 +3017,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B88">
         <f t="shared" si="1"/>
@@ -3025,7 +3027,10 @@
         <v>13</v>
       </c>
       <c r="D88" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="F88" t="s">
+        <v>2</v>
       </c>
       <c r="G88" t="b">
         <v>1</v>
@@ -3036,7 +3041,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B89">
         <f t="shared" si="1"/>
@@ -3046,7 +3051,10 @@
         <v>13</v>
       </c>
       <c r="D89" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="F89" t="s">
+        <v>2</v>
       </c>
       <c r="G89" t="b">
         <v>1</v>
@@ -3057,7 +3065,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B90">
         <f t="shared" si="1"/>
@@ -3067,7 +3075,10 @@
         <v>18</v>
       </c>
       <c r="D90" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="F90" t="s">
+        <v>1</v>
       </c>
       <c r="G90" t="b">
         <v>0</v>
@@ -3078,7 +3089,7 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B91">
         <f t="shared" si="1"/>
@@ -3088,7 +3099,10 @@
         <v>18</v>
       </c>
       <c r="D91" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="F91" t="s">
+        <v>1</v>
       </c>
       <c r="G91" t="b">
         <v>0</v>
@@ -3099,7 +3113,7 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B92">
         <f t="shared" si="1"/>
@@ -3109,7 +3123,10 @@
         <v>18</v>
       </c>
       <c r="D92" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="F92" t="s">
+        <v>1</v>
       </c>
       <c r="G92" t="b">
         <v>0</v>
@@ -3120,7 +3137,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B93">
         <f t="shared" si="1"/>
@@ -3130,7 +3147,7 @@
         <v>18</v>
       </c>
       <c r="D93" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E93" t="s">
         <v>19</v>
@@ -3147,7 +3164,7 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B94">
         <f t="shared" si="1"/>
@@ -3174,7 +3191,7 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B95">
         <f t="shared" si="1"/>
@@ -3184,7 +3201,7 @@
         <v>13</v>
       </c>
       <c r="D95" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F95" t="s">
         <v>1</v>
@@ -3198,7 +3215,7 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B96">
         <f t="shared" si="1"/>
@@ -3208,7 +3225,7 @@
         <v>13</v>
       </c>
       <c r="D96" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F96" t="s">
         <v>2</v>
@@ -3222,7 +3239,7 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B97">
         <f t="shared" si="1"/>
@@ -3232,7 +3249,7 @@
         <v>13</v>
       </c>
       <c r="D97" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F97" t="s">
         <v>2</v>
@@ -3246,7 +3263,7 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B98">
         <f t="shared" si="1"/>
@@ -3256,7 +3273,7 @@
         <v>18</v>
       </c>
       <c r="D98" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F98" t="s">
         <v>1</v>
@@ -3270,7 +3287,7 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B99">
         <f t="shared" si="1"/>
@@ -3280,7 +3297,7 @@
         <v>18</v>
       </c>
       <c r="D99" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F99" t="s">
         <v>1</v>
@@ -3294,7 +3311,7 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B100">
         <f t="shared" si="1"/>
@@ -3304,7 +3321,7 @@
         <v>18</v>
       </c>
       <c r="D100" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F100" t="s">
         <v>1</v>
@@ -3318,7 +3335,7 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B101">
         <f t="shared" si="1"/>
@@ -3328,7 +3345,7 @@
         <v>18</v>
       </c>
       <c r="D101" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E101" t="s">
         <v>19</v>
@@ -3345,7 +3362,7 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B102">
         <f t="shared" si="1"/>
@@ -3372,7 +3389,7 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B103">
         <f t="shared" si="1"/>
@@ -3382,7 +3399,7 @@
         <v>13</v>
       </c>
       <c r="D103" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F103" t="s">
         <v>1</v>
@@ -3396,7 +3413,7 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B104">
         <f t="shared" si="1"/>
@@ -3406,7 +3423,7 @@
         <v>13</v>
       </c>
       <c r="D104" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F104" t="s">
         <v>2</v>
@@ -3420,7 +3437,7 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B105">
         <f t="shared" si="1"/>
@@ -3430,7 +3447,7 @@
         <v>13</v>
       </c>
       <c r="D105" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F105" t="s">
         <v>2</v>
@@ -3444,7 +3461,7 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B106">
         <f t="shared" si="1"/>
@@ -3454,7 +3471,7 @@
         <v>18</v>
       </c>
       <c r="D106" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E106" t="s">
         <v>19</v>
@@ -3471,7 +3488,7 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B107">
         <f t="shared" si="1"/>
@@ -3498,7 +3515,7 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B108">
         <f t="shared" si="1"/>
@@ -3508,7 +3525,7 @@
         <v>13</v>
       </c>
       <c r="D108" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F108" t="s">
         <v>1</v>
@@ -3522,7 +3539,7 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B109">
         <f t="shared" si="1"/>
@@ -3532,7 +3549,7 @@
         <v>13</v>
       </c>
       <c r="D109" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F109" t="s">
         <v>2</v>
@@ -3546,7 +3563,7 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B110">
         <f t="shared" si="1"/>
@@ -3556,7 +3573,7 @@
         <v>13</v>
       </c>
       <c r="D110" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F110" t="s">
         <v>2</v>
@@ -3570,7 +3587,7 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B111">
         <f t="shared" si="1"/>
@@ -3580,7 +3597,7 @@
         <v>18</v>
       </c>
       <c r="D111" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G111" t="b">
         <v>0</v>
@@ -3591,7 +3608,7 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B112">
         <f t="shared" si="1"/>
@@ -3601,7 +3618,7 @@
         <v>18</v>
       </c>
       <c r="D112" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E112" t="s">
         <v>19</v>
@@ -3618,7 +3635,7 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B113">
         <f t="shared" si="1"/>
@@ -3645,7 +3662,7 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B114">
         <f t="shared" si="1"/>
@@ -3655,7 +3672,7 @@
         <v>13</v>
       </c>
       <c r="D114" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F114" t="s">
         <v>1</v>
@@ -3669,7 +3686,7 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B115">
         <f t="shared" si="1"/>
@@ -3679,7 +3696,7 @@
         <v>13</v>
       </c>
       <c r="D115" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F115" t="s">
         <v>2</v>
@@ -3693,7 +3710,7 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B116">
         <f t="shared" si="1"/>
@@ -3703,7 +3720,7 @@
         <v>13</v>
       </c>
       <c r="D116" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F116" t="s">
         <v>2</v>
@@ -3717,7 +3734,7 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B117">
         <f t="shared" si="1"/>
@@ -3727,7 +3744,7 @@
         <v>18</v>
       </c>
       <c r="D117" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F117" t="s">
         <v>1</v>
@@ -3741,7 +3758,7 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B118">
         <f t="shared" si="1"/>
@@ -3751,7 +3768,7 @@
         <v>18</v>
       </c>
       <c r="D118" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F118" t="s">
         <v>1</v>
@@ -3765,7 +3782,7 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B119">
         <f t="shared" si="1"/>
@@ -3775,7 +3792,7 @@
         <v>18</v>
       </c>
       <c r="D119" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F119" t="s">
         <v>1</v>
@@ -3789,7 +3806,7 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B120">
         <f t="shared" si="1"/>
@@ -3799,7 +3816,7 @@
         <v>18</v>
       </c>
       <c r="D120" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E120" t="s">
         <v>19</v>
@@ -3816,7 +3833,7 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B121">
         <f t="shared" si="1"/>
@@ -3843,7 +3860,7 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B122">
         <f t="shared" si="1"/>
@@ -3853,7 +3870,7 @@
         <v>13</v>
       </c>
       <c r="D122" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F122" t="s">
         <v>1</v>
@@ -3867,7 +3884,7 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B123">
         <f t="shared" si="1"/>
@@ -3877,7 +3894,7 @@
         <v>13</v>
       </c>
       <c r="D123" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F123" t="s">
         <v>2</v>
@@ -3891,7 +3908,7 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B124">
         <f t="shared" si="1"/>
@@ -3901,7 +3918,7 @@
         <v>13</v>
       </c>
       <c r="D124" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F124" t="s">
         <v>2</v>
@@ -3915,7 +3932,7 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B125">
         <f t="shared" si="1"/>
@@ -3925,7 +3942,7 @@
         <v>18</v>
       </c>
       <c r="D125" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F125" t="s">
         <v>1</v>
@@ -3939,7 +3956,7 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B126">
         <f t="shared" si="1"/>
@@ -3949,7 +3966,7 @@
         <v>18</v>
       </c>
       <c r="D126" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E126" t="s">
         <v>19</v>
@@ -3966,7 +3983,7 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B127">
         <f t="shared" si="1"/>
@@ -3993,7 +4010,7 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B128">
         <f t="shared" si="1"/>
@@ -4003,7 +4020,7 @@
         <v>13</v>
       </c>
       <c r="D128" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F128" t="s">
         <v>1</v>
@@ -4017,7 +4034,7 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B129">
         <f t="shared" si="1"/>
@@ -4027,7 +4044,7 @@
         <v>13</v>
       </c>
       <c r="D129" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F129" t="s">
         <v>2</v>
@@ -4041,7 +4058,7 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B130">
         <f t="shared" si="1"/>
@@ -4051,7 +4068,7 @@
         <v>13</v>
       </c>
       <c r="D130" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F130" t="s">
         <v>2</v>
@@ -4065,7 +4082,7 @@
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B131">
         <f t="shared" ref="B131:B194" si="2">IF(AND(A130=A131, C130=C131), B130+1, 1)</f>
@@ -4075,7 +4092,7 @@
         <v>18</v>
       </c>
       <c r="D131" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F131" t="s">
         <v>1</v>
@@ -4089,7 +4106,7 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B132">
         <f t="shared" si="2"/>
@@ -4099,7 +4116,7 @@
         <v>18</v>
       </c>
       <c r="D132" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F132" t="s">
         <v>1</v>
@@ -4113,7 +4130,7 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B133">
         <f t="shared" si="2"/>
@@ -4123,7 +4140,7 @@
         <v>18</v>
       </c>
       <c r="D133" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E133" t="s">
         <v>19</v>
@@ -4140,7 +4157,7 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B134">
         <f t="shared" si="2"/>
@@ -4167,7 +4184,7 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B135">
         <f t="shared" si="2"/>
@@ -4177,7 +4194,7 @@
         <v>13</v>
       </c>
       <c r="D135" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F135" t="s">
         <v>1</v>
@@ -4191,7 +4208,7 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B136">
         <f t="shared" si="2"/>
@@ -4201,7 +4218,7 @@
         <v>13</v>
       </c>
       <c r="D136" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F136" t="s">
         <v>2</v>
@@ -4215,7 +4232,7 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B137">
         <f t="shared" si="2"/>
@@ -4225,7 +4242,7 @@
         <v>13</v>
       </c>
       <c r="D137" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F137" t="s">
         <v>2</v>
@@ -4239,7 +4256,7 @@
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B138">
         <f t="shared" si="2"/>
@@ -4249,7 +4266,7 @@
         <v>18</v>
       </c>
       <c r="D138" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F138" t="s">
         <v>1</v>
@@ -4263,7 +4280,7 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B139">
         <f t="shared" si="2"/>
@@ -4273,7 +4290,7 @@
         <v>18</v>
       </c>
       <c r="D139" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F139" t="s">
         <v>1</v>
@@ -4287,7 +4304,7 @@
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B140">
         <f t="shared" si="2"/>
@@ -4297,7 +4314,7 @@
         <v>18</v>
       </c>
       <c r="D140" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F140" t="s">
         <v>1</v>
@@ -4311,7 +4328,7 @@
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B141">
         <f t="shared" si="2"/>
@@ -4321,7 +4338,7 @@
         <v>18</v>
       </c>
       <c r="D141" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F141" t="s">
         <v>1</v>
@@ -4335,7 +4352,7 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B142">
         <f t="shared" si="2"/>
@@ -4345,7 +4362,7 @@
         <v>18</v>
       </c>
       <c r="D142" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F142" t="s">
         <v>1</v>
@@ -4359,7 +4376,7 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B143">
         <f t="shared" si="2"/>
@@ -4369,7 +4386,7 @@
         <v>18</v>
       </c>
       <c r="D143" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E143" t="s">
         <v>19</v>
@@ -4386,7 +4403,7 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B144">
         <f t="shared" si="2"/>
@@ -4413,7 +4430,7 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B145">
         <f t="shared" si="2"/>
@@ -4423,7 +4440,7 @@
         <v>13</v>
       </c>
       <c r="D145" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F145" t="s">
         <v>1</v>
@@ -4437,7 +4454,7 @@
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B146">
         <f t="shared" si="2"/>
@@ -4447,7 +4464,7 @@
         <v>13</v>
       </c>
       <c r="D146" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F146" t="s">
         <v>2</v>
@@ -4461,7 +4478,7 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B147">
         <f t="shared" si="2"/>
@@ -4471,7 +4488,7 @@
         <v>13</v>
       </c>
       <c r="D147" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F147" t="s">
         <v>2</v>
@@ -4485,7 +4502,7 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B148">
         <f t="shared" si="2"/>
@@ -4495,7 +4512,7 @@
         <v>18</v>
       </c>
       <c r="D148" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F148" t="s">
         <v>1</v>
@@ -4509,7 +4526,7 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B149">
         <f t="shared" si="2"/>
@@ -4519,7 +4536,7 @@
         <v>18</v>
       </c>
       <c r="D149" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F149" t="s">
         <v>1</v>
@@ -4533,7 +4550,7 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B150">
         <f t="shared" si="2"/>
@@ -4543,7 +4560,7 @@
         <v>18</v>
       </c>
       <c r="D150" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F150" t="s">
         <v>1</v>
@@ -4557,7 +4574,7 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B151">
         <f t="shared" si="2"/>
@@ -4567,7 +4584,7 @@
         <v>18</v>
       </c>
       <c r="D151" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F151" t="s">
         <v>1</v>
@@ -4581,7 +4598,7 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B152">
         <f t="shared" si="2"/>
@@ -4591,7 +4608,7 @@
         <v>18</v>
       </c>
       <c r="D152" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F152" t="s">
         <v>1</v>
@@ -4605,7 +4622,7 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B153">
         <f t="shared" si="2"/>
@@ -4615,7 +4632,7 @@
         <v>18</v>
       </c>
       <c r="D153" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E153" t="s">
         <v>19</v>
@@ -4632,7 +4649,7 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B154">
         <f t="shared" si="2"/>
@@ -4659,7 +4676,7 @@
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B155">
         <f t="shared" si="2"/>
@@ -4669,7 +4686,7 @@
         <v>13</v>
       </c>
       <c r="D155" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F155" t="s">
         <v>1</v>
@@ -4683,7 +4700,7 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B156">
         <f t="shared" si="2"/>
@@ -4693,7 +4710,7 @@
         <v>13</v>
       </c>
       <c r="D156" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F156" t="s">
         <v>2</v>
@@ -4707,7 +4724,7 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B157">
         <f t="shared" si="2"/>
@@ -4717,7 +4734,7 @@
         <v>13</v>
       </c>
       <c r="D157" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F157" t="s">
         <v>2</v>
@@ -4731,7 +4748,7 @@
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B158">
         <f t="shared" si="2"/>
@@ -4741,7 +4758,7 @@
         <v>18</v>
       </c>
       <c r="D158" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F158" t="s">
         <v>1</v>
@@ -4755,7 +4772,7 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B159">
         <f t="shared" si="2"/>
@@ -4765,7 +4782,7 @@
         <v>18</v>
       </c>
       <c r="D159" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E159" t="s">
         <v>19</v>
@@ -4782,7 +4799,7 @@
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B160">
         <f t="shared" si="2"/>
@@ -4809,7 +4826,7 @@
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B161">
         <f t="shared" si="2"/>
@@ -4819,7 +4836,7 @@
         <v>13</v>
       </c>
       <c r="D161" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F161" t="s">
         <v>1</v>
@@ -4833,7 +4850,7 @@
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B162">
         <f t="shared" si="2"/>
@@ -4843,7 +4860,7 @@
         <v>13</v>
       </c>
       <c r="D162" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F162" t="s">
         <v>2</v>
@@ -4857,7 +4874,7 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B163">
         <f t="shared" si="2"/>
@@ -4867,7 +4884,7 @@
         <v>13</v>
       </c>
       <c r="D163" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F163" t="s">
         <v>2</v>
@@ -4881,7 +4898,7 @@
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B164">
         <f t="shared" si="2"/>
@@ -4891,7 +4908,7 @@
         <v>18</v>
       </c>
       <c r="D164" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F164" t="s">
         <v>1</v>
@@ -4905,7 +4922,7 @@
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B165">
         <f t="shared" si="2"/>
@@ -4915,7 +4932,7 @@
         <v>18</v>
       </c>
       <c r="D165" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E165" t="s">
         <v>19</v>
@@ -4932,7 +4949,7 @@
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B166">
         <f t="shared" si="2"/>
@@ -4959,7 +4976,7 @@
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B167">
         <f t="shared" si="2"/>
@@ -4969,7 +4986,7 @@
         <v>13</v>
       </c>
       <c r="D167" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F167" t="s">
         <v>1</v>
@@ -4983,7 +5000,7 @@
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B168">
         <f t="shared" si="2"/>
@@ -4993,7 +5010,7 @@
         <v>13</v>
       </c>
       <c r="D168" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F168" t="s">
         <v>2</v>
@@ -5007,7 +5024,7 @@
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B169">
         <f t="shared" si="2"/>
@@ -5017,7 +5034,7 @@
         <v>13</v>
       </c>
       <c r="D169" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F169" t="s">
         <v>2</v>
@@ -5031,7 +5048,7 @@
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B170">
         <f t="shared" si="2"/>
@@ -5041,7 +5058,7 @@
         <v>18</v>
       </c>
       <c r="D170" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F170" t="s">
         <v>1</v>
@@ -5055,7 +5072,7 @@
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B171">
         <f t="shared" si="2"/>
@@ -5065,7 +5082,7 @@
         <v>18</v>
       </c>
       <c r="D171" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E171" t="s">
         <v>19</v>
@@ -5082,7 +5099,7 @@
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B172">
         <f t="shared" si="2"/>
@@ -5109,7 +5126,7 @@
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B173">
         <f t="shared" si="2"/>
@@ -5119,7 +5136,7 @@
         <v>13</v>
       </c>
       <c r="D173" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F173" t="s">
         <v>1</v>
@@ -5133,7 +5150,7 @@
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B174">
         <f t="shared" si="2"/>
@@ -5143,7 +5160,7 @@
         <v>13</v>
       </c>
       <c r="D174" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F174" t="s">
         <v>2</v>
@@ -5157,7 +5174,7 @@
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B175">
         <f t="shared" si="2"/>
@@ -5167,7 +5184,7 @@
         <v>13</v>
       </c>
       <c r="D175" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F175" t="s">
         <v>2</v>
@@ -5181,7 +5198,7 @@
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B176">
         <f t="shared" si="2"/>
@@ -5191,7 +5208,7 @@
         <v>18</v>
       </c>
       <c r="D176" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F176" t="s">
         <v>1</v>
@@ -5205,7 +5222,7 @@
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B177">
         <f t="shared" si="2"/>
@@ -5215,7 +5232,7 @@
         <v>18</v>
       </c>
       <c r="D177" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F177" t="s">
         <v>1</v>
@@ -5229,7 +5246,7 @@
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B178">
         <f t="shared" si="2"/>
@@ -5239,7 +5256,7 @@
         <v>18</v>
       </c>
       <c r="D178" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E178" t="s">
         <v>19</v>
@@ -5256,7 +5273,7 @@
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B179">
         <f t="shared" si="2"/>
@@ -5283,7 +5300,7 @@
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B180">
         <f t="shared" si="2"/>
@@ -5293,7 +5310,7 @@
         <v>13</v>
       </c>
       <c r="D180" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F180" t="s">
         <v>1</v>
@@ -5307,7 +5324,7 @@
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B181">
         <f t="shared" si="2"/>
@@ -5317,7 +5334,7 @@
         <v>13</v>
       </c>
       <c r="D181" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F181" t="s">
         <v>2</v>
@@ -5331,7 +5348,7 @@
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B182">
         <f t="shared" si="2"/>
@@ -5341,7 +5358,7 @@
         <v>13</v>
       </c>
       <c r="D182" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F182" t="s">
         <v>2</v>
@@ -5355,7 +5372,7 @@
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B183">
         <f t="shared" si="2"/>
@@ -5365,7 +5382,7 @@
         <v>18</v>
       </c>
       <c r="D183" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F183" t="s">
         <v>1</v>
@@ -5379,7 +5396,7 @@
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B184">
         <f t="shared" si="2"/>
@@ -5389,7 +5406,7 @@
         <v>18</v>
       </c>
       <c r="D184" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F184" t="s">
         <v>1</v>
@@ -5403,7 +5420,7 @@
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B185">
         <f t="shared" si="2"/>
@@ -5413,7 +5430,7 @@
         <v>18</v>
       </c>
       <c r="D185" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F185" t="s">
         <v>1</v>
@@ -5427,7 +5444,7 @@
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B186">
         <f t="shared" si="2"/>
@@ -5437,7 +5454,7 @@
         <v>18</v>
       </c>
       <c r="D186" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F186" t="s">
         <v>1</v>
@@ -5451,7 +5468,7 @@
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B187">
         <f t="shared" si="2"/>
@@ -5461,7 +5478,7 @@
         <v>18</v>
       </c>
       <c r="D187" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E187" t="s">
         <v>19</v>
@@ -5478,7 +5495,7 @@
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B188">
         <f t="shared" si="2"/>
@@ -5505,7 +5522,7 @@
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B189">
         <f t="shared" si="2"/>
@@ -5515,7 +5532,7 @@
         <v>13</v>
       </c>
       <c r="D189" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F189" t="s">
         <v>1</v>
@@ -5529,7 +5546,7 @@
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B190">
         <f t="shared" si="2"/>
@@ -5539,7 +5556,7 @@
         <v>13</v>
       </c>
       <c r="D190" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F190" t="s">
         <v>2</v>
@@ -5553,7 +5570,7 @@
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B191">
         <f t="shared" si="2"/>
@@ -5563,7 +5580,7 @@
         <v>13</v>
       </c>
       <c r="D191" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F191" t="s">
         <v>2</v>
@@ -5577,7 +5594,7 @@
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B192">
         <f t="shared" si="2"/>
@@ -5587,7 +5604,7 @@
         <v>18</v>
       </c>
       <c r="D192" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F192" t="s">
         <v>1</v>
@@ -5601,7 +5618,7 @@
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B193">
         <f t="shared" si="2"/>
@@ -5611,7 +5628,7 @@
         <v>18</v>
       </c>
       <c r="D193" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F193" t="s">
         <v>1</v>
@@ -5625,7 +5642,7 @@
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B194">
         <f t="shared" si="2"/>
@@ -5635,7 +5652,7 @@
         <v>18</v>
       </c>
       <c r="D194" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F194" t="s">
         <v>1</v>
@@ -5649,7 +5666,7 @@
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B195">
         <f t="shared" ref="B195:B225" si="3">IF(AND(A194=A195, C194=C195), B194+1, 1)</f>
@@ -5659,7 +5676,7 @@
         <v>18</v>
       </c>
       <c r="D195" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F195" t="s">
         <v>1</v>
@@ -5673,7 +5690,7 @@
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B196">
         <f t="shared" si="3"/>
@@ -5683,7 +5700,7 @@
         <v>18</v>
       </c>
       <c r="D196" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E196" t="s">
         <v>19</v>
@@ -5700,7 +5717,7 @@
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B197">
         <f t="shared" si="3"/>
@@ -5727,7 +5744,7 @@
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B198">
         <f t="shared" si="3"/>
@@ -5737,7 +5754,7 @@
         <v>13</v>
       </c>
       <c r="D198" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F198" t="s">
         <v>1</v>
@@ -5751,7 +5768,7 @@
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B199">
         <f t="shared" si="3"/>
@@ -5761,7 +5778,7 @@
         <v>13</v>
       </c>
       <c r="D199" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F199" t="s">
         <v>2</v>
@@ -5775,7 +5792,7 @@
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B200">
         <f t="shared" si="3"/>
@@ -5785,7 +5802,7 @@
         <v>13</v>
       </c>
       <c r="D200" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F200" t="s">
         <v>2</v>
@@ -5799,7 +5816,7 @@
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B201">
         <f t="shared" si="3"/>
@@ -5809,7 +5826,7 @@
         <v>18</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F201" t="s">
         <v>1</v>
@@ -5823,7 +5840,7 @@
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B202">
         <f t="shared" si="3"/>
@@ -5833,7 +5850,7 @@
         <v>18</v>
       </c>
       <c r="D202" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E202" t="s">
         <v>19</v>
@@ -5850,7 +5867,7 @@
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B203">
         <f t="shared" si="3"/>
@@ -5877,7 +5894,7 @@
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B204">
         <f t="shared" si="3"/>
@@ -5887,7 +5904,7 @@
         <v>13</v>
       </c>
       <c r="D204" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F204" t="s">
         <v>1</v>
@@ -5901,7 +5918,7 @@
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B205">
         <f t="shared" si="3"/>
@@ -5911,7 +5928,7 @@
         <v>13</v>
       </c>
       <c r="D205" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F205" t="s">
         <v>2</v>
@@ -5925,7 +5942,7 @@
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B206">
         <f t="shared" si="3"/>
@@ -5935,7 +5952,7 @@
         <v>13</v>
       </c>
       <c r="D206" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F206" t="s">
         <v>2</v>
@@ -5949,7 +5966,7 @@
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B207">
         <f t="shared" si="3"/>
@@ -5959,7 +5976,7 @@
         <v>18</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F207" t="s">
         <v>1</v>
@@ -5973,7 +5990,7 @@
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B208">
         <f t="shared" si="3"/>
@@ -5983,7 +6000,7 @@
         <v>18</v>
       </c>
       <c r="D208" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E208" t="s">
         <v>19</v>
@@ -6000,7 +6017,7 @@
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B209">
         <f t="shared" si="3"/>
@@ -6027,7 +6044,7 @@
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B210">
         <f t="shared" si="3"/>
@@ -6037,7 +6054,7 @@
         <v>13</v>
       </c>
       <c r="D210" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F210" t="s">
         <v>1</v>
@@ -6051,7 +6068,7 @@
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B211">
         <f t="shared" si="3"/>
@@ -6061,7 +6078,7 @@
         <v>13</v>
       </c>
       <c r="D211" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F211" t="s">
         <v>2</v>
@@ -6075,7 +6092,7 @@
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B212">
         <f t="shared" si="3"/>
@@ -6085,7 +6102,7 @@
         <v>13</v>
       </c>
       <c r="D212" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F212" t="s">
         <v>2</v>
@@ -6099,7 +6116,7 @@
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B213">
         <f t="shared" si="3"/>
@@ -6109,7 +6126,7 @@
         <v>18</v>
       </c>
       <c r="D213" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F213" t="s">
         <v>1</v>
@@ -6123,7 +6140,7 @@
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B214">
         <f t="shared" si="3"/>
@@ -6133,7 +6150,7 @@
         <v>18</v>
       </c>
       <c r="D214" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E214" t="s">
         <v>19</v>
@@ -6150,7 +6167,7 @@
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B215">
         <f t="shared" si="3"/>
@@ -6177,7 +6194,7 @@
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B216">
         <f t="shared" si="3"/>
@@ -6187,7 +6204,7 @@
         <v>13</v>
       </c>
       <c r="D216" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F216" t="s">
         <v>1</v>
@@ -6201,7 +6218,7 @@
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B217">
         <f t="shared" si="3"/>
@@ -6211,7 +6228,7 @@
         <v>13</v>
       </c>
       <c r="D217" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F217" t="s">
         <v>2</v>
@@ -6225,7 +6242,7 @@
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B218">
         <f t="shared" si="3"/>
@@ -6235,7 +6252,7 @@
         <v>13</v>
       </c>
       <c r="D218" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F218" t="s">
         <v>2</v>
@@ -6249,7 +6266,7 @@
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B219">
         <f t="shared" si="3"/>
@@ -6259,7 +6276,7 @@
         <v>18</v>
       </c>
       <c r="D219" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E219" t="s">
         <v>19</v>
@@ -6276,7 +6293,7 @@
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B220">
         <f t="shared" si="3"/>
@@ -6303,7 +6320,7 @@
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B221">
         <f t="shared" si="3"/>
@@ -6313,7 +6330,7 @@
         <v>13</v>
       </c>
       <c r="D221" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F221" t="s">
         <v>1</v>
@@ -6327,7 +6344,7 @@
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B222">
         <f t="shared" si="3"/>
@@ -6337,7 +6354,7 @@
         <v>13</v>
       </c>
       <c r="D222" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F222" t="s">
         <v>2</v>
@@ -6351,7 +6368,7 @@
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B223">
         <f t="shared" si="3"/>
@@ -6361,7 +6378,7 @@
         <v>13</v>
       </c>
       <c r="D223" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F223" t="s">
         <v>2</v>
@@ -6375,7 +6392,7 @@
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B224">
         <f t="shared" si="3"/>
@@ -6385,7 +6402,7 @@
         <v>18</v>
       </c>
       <c r="D224" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F224" t="s">
         <v>1</v>
@@ -6399,7 +6416,7 @@
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B225">
         <f t="shared" si="3"/>
@@ -6409,7 +6426,7 @@
         <v>18</v>
       </c>
       <c r="D225" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="E225" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Repeated Measures Anaylsis - closes #31
</commit_message>
<xml_diff>
--- a/scripts/table_examples/titles.xlsx
+++ b/scripts/table_examples/titles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16105\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89460901-7272-434E-8B62-C146B3A73170}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1F7503-4F40-4DAB-A1A4-2D5A6B0A5ED2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{45CA4081-01D7-4010-B007-0BB33FDF9BEF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{45CA4081-01D7-4010-B007-0BB33FDF9BEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="149">
   <si>
     <t>split</t>
   </si>
@@ -837,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278D11AC-8C4C-4475-BF03-113D4886E6A9}">
   <dimension ref="A1:I225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
-      <selection activeCell="F224" sqref="F224"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="F111" sqref="F111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3599,6 +3599,9 @@
       <c r="D111" t="s">
         <v>79</v>
       </c>
+      <c r="F111" t="s">
+        <v>1</v>
+      </c>
       <c r="G111" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Updated for Ashley's comments.
</commit_message>
<xml_diff>
--- a/scripts/table_examples/titles.xlsx
+++ b/scripts/table_examples/titles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16105\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16105\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1F7503-4F40-4DAB-A1A4-2D5A6B0A5ED2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17321217-2421-4CCC-B630-B301DCDE657C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{45CA4081-01D7-4010-B007-0BB33FDF9BEF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{45CA4081-01D7-4010-B007-0BB33FDF9BEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="148">
   <si>
     <t>split</t>
   </si>
@@ -162,9 +162,6 @@
   </si>
   <si>
     <t>[2] Test for a non-zero coefficient for treatment (dose) as a continuous variable</t>
-  </si>
-  <si>
-    <t>[3] Pairwise comparison with treatment as a categorical variable: p-values without adjustment for multiplec omparisons.</t>
   </si>
   <si>
     <t>[1] Based on Analysis of covariance (ANCOVA) model with treatment and site group as factors and baseline value as a covariate.</t>
@@ -835,10 +832,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278D11AC-8C4C-4475-BF03-113D4886E6A9}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="F111" sqref="F111"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,7 +856,7 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
@@ -882,7 +880,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -909,7 +907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -933,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -957,7 +955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -981,7 +979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1005,7 +1003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1017,7 +1015,7 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
@@ -1032,7 +1030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1059,7 +1057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1083,7 +1081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1107,7 +1105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1131,7 +1129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1155,7 +1153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1179,7 +1177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1191,7 +1189,7 @@
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E14" t="s">
         <v>19</v>
@@ -1206,7 +1204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1233,7 +1231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1257,7 +1255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1281,7 +1279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1305,7 +1303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1329,7 +1327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1353,7 +1351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1365,7 +1363,7 @@
         <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E21" t="s">
         <v>19</v>
@@ -1380,7 +1378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1407,7 +1405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1431,7 +1429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1455,7 +1453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1479,7 +1477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1503,7 +1501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1527,7 +1525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1539,7 +1537,7 @@
         <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E28" t="s">
         <v>19</v>
@@ -1665,7 +1663,7 @@
         <v>18</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F33" t="s">
         <v>1</v>
@@ -1713,7 +1711,7 @@
         <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F35" t="s">
         <v>1</v>
@@ -1737,7 +1735,7 @@
         <v>18</v>
       </c>
       <c r="D36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E36" t="s">
         <v>19</v>
@@ -1752,9 +1750,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
@@ -1779,9 +1777,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
@@ -1803,9 +1801,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
@@ -1815,7 +1813,7 @@
         <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F39" t="s">
         <v>2</v>
@@ -1827,9 +1825,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B40">
         <f t="shared" si="0"/>
@@ -1839,7 +1837,7 @@
         <v>13</v>
       </c>
       <c r="D40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F40" t="s">
         <v>2</v>
@@ -1851,9 +1849,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
@@ -1863,7 +1861,7 @@
         <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F41" t="s">
         <v>1</v>
@@ -1875,9 +1873,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42">
         <f t="shared" si="0"/>
@@ -1887,7 +1885,7 @@
         <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F42" t="s">
         <v>1</v>
@@ -1899,9 +1897,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43">
         <f t="shared" si="0"/>
@@ -1911,7 +1909,7 @@
         <v>18</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F43" t="s">
         <v>1</v>
@@ -1923,9 +1921,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44">
         <f t="shared" si="0"/>
@@ -1935,7 +1933,7 @@
         <v>18</v>
       </c>
       <c r="D44" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E44" t="s">
         <v>19</v>
@@ -1950,9 +1948,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B45">
         <f t="shared" si="0"/>
@@ -1977,9 +1975,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B46">
         <f t="shared" si="0"/>
@@ -2001,9 +1999,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B47">
         <f t="shared" si="0"/>
@@ -2013,7 +2011,7 @@
         <v>13</v>
       </c>
       <c r="D47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F47" t="s">
         <v>2</v>
@@ -2025,9 +2023,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B48">
         <f t="shared" si="0"/>
@@ -2037,7 +2035,7 @@
         <v>13</v>
       </c>
       <c r="D48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F48" t="s">
         <v>2</v>
@@ -2049,9 +2047,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49">
         <f t="shared" si="0"/>
@@ -2061,7 +2059,7 @@
         <v>18</v>
       </c>
       <c r="D49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F49" t="s">
         <v>1</v>
@@ -2073,9 +2071,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50">
         <f t="shared" si="0"/>
@@ -2085,7 +2083,7 @@
         <v>18</v>
       </c>
       <c r="D50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F50" t="s">
         <v>1</v>
@@ -2097,9 +2095,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51">
         <f t="shared" si="0"/>
@@ -2109,21 +2107,21 @@
         <v>18</v>
       </c>
       <c r="D51" t="s">
+        <v>48</v>
+      </c>
+      <c r="F51" t="s">
+        <v>1</v>
+      </c>
+      <c r="G51" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>49</v>
-      </c>
-      <c r="F51" t="s">
-        <v>1</v>
-      </c>
-      <c r="G51" t="b">
-        <v>0</v>
-      </c>
-      <c r="H51" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>50</v>
       </c>
       <c r="B52">
         <f t="shared" si="0"/>
@@ -2133,7 +2131,7 @@
         <v>18</v>
       </c>
       <c r="D52" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E52" t="s">
         <v>19</v>
@@ -2148,9 +2146,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53">
         <f t="shared" si="0"/>
@@ -2175,9 +2173,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54">
         <f t="shared" si="0"/>
@@ -2199,9 +2197,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55">
         <f t="shared" si="0"/>
@@ -2211,7 +2209,7 @@
         <v>13</v>
       </c>
       <c r="D55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F55" t="s">
         <v>2</v>
@@ -2223,9 +2221,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B56">
         <f t="shared" si="0"/>
@@ -2235,7 +2233,7 @@
         <v>13</v>
       </c>
       <c r="D56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F56" t="s">
         <v>2</v>
@@ -2247,9 +2245,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B57">
         <f t="shared" si="0"/>
@@ -2259,7 +2257,7 @@
         <v>18</v>
       </c>
       <c r="D57" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F57" t="s">
         <v>1</v>
@@ -2271,9 +2269,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B58">
         <f t="shared" si="0"/>
@@ -2283,7 +2281,7 @@
         <v>18</v>
       </c>
       <c r="D58" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F58" t="s">
         <v>1</v>
@@ -2295,9 +2293,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B59">
         <f t="shared" si="0"/>
@@ -2307,7 +2305,7 @@
         <v>18</v>
       </c>
       <c r="D59" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F59" t="s">
         <v>1</v>
@@ -2319,9 +2317,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B60">
         <f t="shared" si="0"/>
@@ -2331,7 +2329,7 @@
         <v>18</v>
       </c>
       <c r="D60" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E60" t="s">
         <v>19</v>
@@ -2346,9 +2344,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B61">
         <f t="shared" si="0"/>
@@ -2373,9 +2371,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B62">
         <f t="shared" si="0"/>
@@ -2397,9 +2395,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B63">
         <f t="shared" si="0"/>
@@ -2409,7 +2407,7 @@
         <v>13</v>
       </c>
       <c r="D63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F63" t="s">
         <v>2</v>
@@ -2421,9 +2419,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B64">
         <f t="shared" si="0"/>
@@ -2433,7 +2431,7 @@
         <v>13</v>
       </c>
       <c r="D64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F64" t="s">
         <v>2</v>
@@ -2445,9 +2443,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B65">
         <f t="shared" si="0"/>
@@ -2457,7 +2455,7 @@
         <v>18</v>
       </c>
       <c r="D65" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F65" t="s">
         <v>1</v>
@@ -2469,9 +2467,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B66">
         <f t="shared" si="0"/>
@@ -2481,7 +2479,7 @@
         <v>18</v>
       </c>
       <c r="D66" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F66" t="s">
         <v>1</v>
@@ -2493,9 +2491,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B67">
         <f t="shared" ref="B67:B130" si="1">IF(AND(A66=A67, C66=C67), B66+1, 1)</f>
@@ -2505,7 +2503,7 @@
         <v>18</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F67" t="s">
         <v>1</v>
@@ -2517,9 +2515,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B68">
         <f t="shared" si="1"/>
@@ -2529,7 +2527,7 @@
         <v>18</v>
       </c>
       <c r="D68" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E68" t="s">
         <v>19</v>
@@ -2544,9 +2542,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B69">
         <f t="shared" si="1"/>
@@ -2571,9 +2569,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B70">
         <f t="shared" si="1"/>
@@ -2595,9 +2593,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B71">
         <f t="shared" si="1"/>
@@ -2607,7 +2605,7 @@
         <v>13</v>
       </c>
       <c r="D71" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F71" t="s">
         <v>2</v>
@@ -2619,9 +2617,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B72">
         <f t="shared" si="1"/>
@@ -2631,7 +2629,7 @@
         <v>13</v>
       </c>
       <c r="D72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F72" t="s">
         <v>2</v>
@@ -2643,9 +2641,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B73">
         <f t="shared" si="1"/>
@@ -2655,7 +2653,7 @@
         <v>18</v>
       </c>
       <c r="D73" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F73" t="s">
         <v>1</v>
@@ -2667,9 +2665,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B74">
         <f t="shared" si="1"/>
@@ -2679,7 +2677,7 @@
         <v>18</v>
       </c>
       <c r="D74" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F74" t="s">
         <v>1</v>
@@ -2691,9 +2689,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B75">
         <f t="shared" si="1"/>
@@ -2703,7 +2701,7 @@
         <v>18</v>
       </c>
       <c r="D75" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F75" t="s">
         <v>1</v>
@@ -2715,9 +2713,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B76">
         <f t="shared" si="1"/>
@@ -2727,7 +2725,7 @@
         <v>18</v>
       </c>
       <c r="D76" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E76" t="s">
         <v>19</v>
@@ -2742,9 +2740,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B77">
         <f t="shared" si="1"/>
@@ -2769,9 +2767,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B78">
         <f t="shared" si="1"/>
@@ -2781,7 +2779,7 @@
         <v>13</v>
       </c>
       <c r="D78" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F78" t="s">
         <v>1</v>
@@ -2793,9 +2791,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B79">
         <f t="shared" si="1"/>
@@ -2805,7 +2803,7 @@
         <v>13</v>
       </c>
       <c r="D79" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F79" t="s">
         <v>2</v>
@@ -2817,9 +2815,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B80">
         <f t="shared" si="1"/>
@@ -2829,7 +2827,7 @@
         <v>13</v>
       </c>
       <c r="D80" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F80" t="s">
         <v>2</v>
@@ -2841,9 +2839,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B81">
         <f t="shared" si="1"/>
@@ -2853,7 +2851,7 @@
         <v>18</v>
       </c>
       <c r="D81" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F81" t="s">
         <v>1</v>
@@ -2865,9 +2863,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B82">
         <f t="shared" si="1"/>
@@ -2877,7 +2875,7 @@
         <v>18</v>
       </c>
       <c r="D82" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F82" t="s">
         <v>1</v>
@@ -2889,9 +2887,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B83">
         <f t="shared" si="1"/>
@@ -2901,7 +2899,7 @@
         <v>18</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F83" t="s">
         <v>1</v>
@@ -2913,9 +2911,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B84">
         <f t="shared" si="1"/>
@@ -2925,7 +2923,7 @@
         <v>18</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F84" t="s">
         <v>1</v>
@@ -2937,9 +2935,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B85">
         <f t="shared" si="1"/>
@@ -2949,7 +2947,7 @@
         <v>18</v>
       </c>
       <c r="D85" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E85" t="s">
         <v>19</v>
@@ -2964,9 +2962,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B86">
         <f t="shared" si="1"/>
@@ -2991,9 +2989,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B87">
         <f t="shared" si="1"/>
@@ -3015,9 +3013,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B88">
         <f t="shared" si="1"/>
@@ -3027,7 +3025,7 @@
         <v>13</v>
       </c>
       <c r="D88" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F88" t="s">
         <v>2</v>
@@ -3039,9 +3037,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B89">
         <f t="shared" si="1"/>
@@ -3051,7 +3049,7 @@
         <v>13</v>
       </c>
       <c r="D89" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F89" t="s">
         <v>2</v>
@@ -3063,9 +3061,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B90">
         <f t="shared" si="1"/>
@@ -3075,7 +3073,7 @@
         <v>18</v>
       </c>
       <c r="D90" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F90" t="s">
         <v>1</v>
@@ -3087,9 +3085,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B91">
         <f t="shared" si="1"/>
@@ -3099,7 +3097,7 @@
         <v>18</v>
       </c>
       <c r="D91" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F91" t="s">
         <v>1</v>
@@ -3111,9 +3109,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B92">
         <f t="shared" si="1"/>
@@ -3123,7 +3121,7 @@
         <v>18</v>
       </c>
       <c r="D92" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F92" t="s">
         <v>1</v>
@@ -3135,9 +3133,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B93">
         <f t="shared" si="1"/>
@@ -3147,7 +3145,7 @@
         <v>18</v>
       </c>
       <c r="D93" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E93" t="s">
         <v>19</v>
@@ -3162,9 +3160,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B94">
         <f t="shared" si="1"/>
@@ -3189,9 +3187,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B95">
         <f t="shared" si="1"/>
@@ -3213,9 +3211,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B96">
         <f t="shared" si="1"/>
@@ -3225,7 +3223,7 @@
         <v>13</v>
       </c>
       <c r="D96" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F96" t="s">
         <v>2</v>
@@ -3237,9 +3235,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B97">
         <f t="shared" si="1"/>
@@ -3249,7 +3247,7 @@
         <v>13</v>
       </c>
       <c r="D97" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F97" t="s">
         <v>2</v>
@@ -3261,9 +3259,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B98">
         <f t="shared" si="1"/>
@@ -3273,7 +3271,7 @@
         <v>18</v>
       </c>
       <c r="D98" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F98" t="s">
         <v>1</v>
@@ -3285,9 +3283,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B99">
         <f t="shared" si="1"/>
@@ -3297,7 +3295,7 @@
         <v>18</v>
       </c>
       <c r="D99" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F99" t="s">
         <v>1</v>
@@ -3309,9 +3307,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B100">
         <f t="shared" si="1"/>
@@ -3321,7 +3319,7 @@
         <v>18</v>
       </c>
       <c r="D100" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F100" t="s">
         <v>1</v>
@@ -3333,9 +3331,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B101">
         <f t="shared" si="1"/>
@@ -3345,7 +3343,7 @@
         <v>18</v>
       </c>
       <c r="D101" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E101" t="s">
         <v>19</v>
@@ -3360,9 +3358,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B102">
         <f t="shared" si="1"/>
@@ -3387,9 +3385,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B103">
         <f t="shared" si="1"/>
@@ -3411,9 +3409,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B104">
         <f t="shared" si="1"/>
@@ -3423,7 +3421,7 @@
         <v>13</v>
       </c>
       <c r="D104" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F104" t="s">
         <v>2</v>
@@ -3435,9 +3433,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B105">
         <f t="shared" si="1"/>
@@ -3447,7 +3445,7 @@
         <v>13</v>
       </c>
       <c r="D105" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F105" t="s">
         <v>2</v>
@@ -3459,9 +3457,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B106">
         <f t="shared" si="1"/>
@@ -3471,7 +3469,7 @@
         <v>18</v>
       </c>
       <c r="D106" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E106" t="s">
         <v>19</v>
@@ -3486,9 +3484,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B107">
         <f t="shared" si="1"/>
@@ -3513,9 +3511,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B108">
         <f t="shared" si="1"/>
@@ -3537,9 +3535,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B109">
         <f t="shared" si="1"/>
@@ -3549,7 +3547,7 @@
         <v>13</v>
       </c>
       <c r="D109" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F109" t="s">
         <v>2</v>
@@ -3561,9 +3559,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B110">
         <f t="shared" si="1"/>
@@ -3573,7 +3571,7 @@
         <v>13</v>
       </c>
       <c r="D110" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F110" t="s">
         <v>2</v>
@@ -3585,9 +3583,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B111">
         <f t="shared" si="1"/>
@@ -3597,7 +3595,7 @@
         <v>18</v>
       </c>
       <c r="D111" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F111" t="s">
         <v>1</v>
@@ -3609,9 +3607,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B112">
         <f t="shared" si="1"/>
@@ -3621,7 +3619,7 @@
         <v>18</v>
       </c>
       <c r="D112" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E112" t="s">
         <v>19</v>
@@ -3636,9 +3634,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B113">
         <f t="shared" si="1"/>
@@ -3663,9 +3661,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B114">
         <f t="shared" si="1"/>
@@ -3687,9 +3685,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B115">
         <f t="shared" si="1"/>
@@ -3699,7 +3697,7 @@
         <v>13</v>
       </c>
       <c r="D115" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F115" t="s">
         <v>2</v>
@@ -3711,9 +3709,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B116">
         <f t="shared" si="1"/>
@@ -3723,7 +3721,7 @@
         <v>13</v>
       </c>
       <c r="D116" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F116" t="s">
         <v>2</v>
@@ -3735,9 +3733,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B117">
         <f t="shared" si="1"/>
@@ -3747,7 +3745,7 @@
         <v>18</v>
       </c>
       <c r="D117" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F117" t="s">
         <v>1</v>
@@ -3759,9 +3757,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B118">
         <f t="shared" si="1"/>
@@ -3771,7 +3769,7 @@
         <v>18</v>
       </c>
       <c r="D118" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F118" t="s">
         <v>1</v>
@@ -3783,9 +3781,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B119">
         <f t="shared" si="1"/>
@@ -3795,7 +3793,7 @@
         <v>18</v>
       </c>
       <c r="D119" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F119" t="s">
         <v>1</v>
@@ -3807,9 +3805,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B120">
         <f t="shared" si="1"/>
@@ -3819,7 +3817,7 @@
         <v>18</v>
       </c>
       <c r="D120" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E120" t="s">
         <v>19</v>
@@ -3834,9 +3832,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B121">
         <f t="shared" si="1"/>
@@ -3861,9 +3859,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B122">
         <f t="shared" si="1"/>
@@ -3885,9 +3883,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B123">
         <f t="shared" si="1"/>
@@ -3897,7 +3895,7 @@
         <v>13</v>
       </c>
       <c r="D123" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F123" t="s">
         <v>2</v>
@@ -3909,9 +3907,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B124">
         <f t="shared" si="1"/>
@@ -3921,7 +3919,7 @@
         <v>13</v>
       </c>
       <c r="D124" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F124" t="s">
         <v>2</v>
@@ -3933,9 +3931,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B125">
         <f t="shared" si="1"/>
@@ -3945,7 +3943,7 @@
         <v>18</v>
       </c>
       <c r="D125" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F125" t="s">
         <v>1</v>
@@ -3957,9 +3955,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B126">
         <f t="shared" si="1"/>
@@ -3969,7 +3967,7 @@
         <v>18</v>
       </c>
       <c r="D126" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E126" t="s">
         <v>19</v>
@@ -3984,9 +3982,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B127">
         <f t="shared" si="1"/>
@@ -4011,9 +4009,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B128">
         <f t="shared" si="1"/>
@@ -4023,7 +4021,7 @@
         <v>13</v>
       </c>
       <c r="D128" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F128" t="s">
         <v>1</v>
@@ -4035,9 +4033,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B129">
         <f t="shared" si="1"/>
@@ -4047,7 +4045,7 @@
         <v>13</v>
       </c>
       <c r="D129" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F129" t="s">
         <v>2</v>
@@ -4059,9 +4057,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B130">
         <f t="shared" si="1"/>
@@ -4071,7 +4069,7 @@
         <v>13</v>
       </c>
       <c r="D130" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F130" t="s">
         <v>2</v>
@@ -4083,9 +4081,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B131">
         <f t="shared" ref="B131:B194" si="2">IF(AND(A130=A131, C130=C131), B130+1, 1)</f>
@@ -4095,7 +4093,7 @@
         <v>18</v>
       </c>
       <c r="D131" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F131" t="s">
         <v>1</v>
@@ -4107,9 +4105,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B132">
         <f t="shared" si="2"/>
@@ -4119,7 +4117,7 @@
         <v>18</v>
       </c>
       <c r="D132" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F132" t="s">
         <v>1</v>
@@ -4131,9 +4129,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B133">
         <f t="shared" si="2"/>
@@ -4143,7 +4141,7 @@
         <v>18</v>
       </c>
       <c r="D133" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E133" t="s">
         <v>19</v>
@@ -4158,9 +4156,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B134">
         <f t="shared" si="2"/>
@@ -4185,9 +4183,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B135">
         <f t="shared" si="2"/>
@@ -4197,7 +4195,7 @@
         <v>13</v>
       </c>
       <c r="D135" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F135" t="s">
         <v>1</v>
@@ -4209,9 +4207,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B136">
         <f t="shared" si="2"/>
@@ -4221,7 +4219,7 @@
         <v>13</v>
       </c>
       <c r="D136" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F136" t="s">
         <v>2</v>
@@ -4233,9 +4231,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B137">
         <f t="shared" si="2"/>
@@ -4245,7 +4243,7 @@
         <v>13</v>
       </c>
       <c r="D137" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F137" t="s">
         <v>2</v>
@@ -4257,9 +4255,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B138">
         <f t="shared" si="2"/>
@@ -4269,7 +4267,7 @@
         <v>18</v>
       </c>
       <c r="D138" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F138" t="s">
         <v>1</v>
@@ -4281,9 +4279,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B139">
         <f t="shared" si="2"/>
@@ -4293,7 +4291,7 @@
         <v>18</v>
       </c>
       <c r="D139" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F139" t="s">
         <v>1</v>
@@ -4305,9 +4303,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B140">
         <f t="shared" si="2"/>
@@ -4317,7 +4315,7 @@
         <v>18</v>
       </c>
       <c r="D140" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F140" t="s">
         <v>1</v>
@@ -4329,9 +4327,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B141">
         <f t="shared" si="2"/>
@@ -4341,7 +4339,7 @@
         <v>18</v>
       </c>
       <c r="D141" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F141" t="s">
         <v>1</v>
@@ -4353,9 +4351,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B142">
         <f t="shared" si="2"/>
@@ -4365,7 +4363,7 @@
         <v>18</v>
       </c>
       <c r="D142" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F142" t="s">
         <v>1</v>
@@ -4377,9 +4375,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B143">
         <f t="shared" si="2"/>
@@ -4389,7 +4387,7 @@
         <v>18</v>
       </c>
       <c r="D143" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E143" t="s">
         <v>19</v>
@@ -4404,9 +4402,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B144">
         <f t="shared" si="2"/>
@@ -4431,9 +4429,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B145">
         <f t="shared" si="2"/>
@@ -4443,7 +4441,7 @@
         <v>13</v>
       </c>
       <c r="D145" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F145" t="s">
         <v>1</v>
@@ -4455,9 +4453,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B146">
         <f t="shared" si="2"/>
@@ -4467,7 +4465,7 @@
         <v>13</v>
       </c>
       <c r="D146" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F146" t="s">
         <v>2</v>
@@ -4479,9 +4477,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B147">
         <f t="shared" si="2"/>
@@ -4491,7 +4489,7 @@
         <v>13</v>
       </c>
       <c r="D147" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F147" t="s">
         <v>2</v>
@@ -4503,9 +4501,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B148">
         <f t="shared" si="2"/>
@@ -4515,7 +4513,7 @@
         <v>18</v>
       </c>
       <c r="D148" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F148" t="s">
         <v>1</v>
@@ -4527,9 +4525,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B149">
         <f t="shared" si="2"/>
@@ -4539,7 +4537,7 @@
         <v>18</v>
       </c>
       <c r="D149" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F149" t="s">
         <v>1</v>
@@ -4551,9 +4549,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B150">
         <f t="shared" si="2"/>
@@ -4563,7 +4561,7 @@
         <v>18</v>
       </c>
       <c r="D150" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F150" t="s">
         <v>1</v>
@@ -4575,9 +4573,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B151">
         <f t="shared" si="2"/>
@@ -4587,7 +4585,7 @@
         <v>18</v>
       </c>
       <c r="D151" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F151" t="s">
         <v>1</v>
@@ -4599,9 +4597,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B152">
         <f t="shared" si="2"/>
@@ -4611,21 +4609,21 @@
         <v>18</v>
       </c>
       <c r="D152" t="s">
+        <v>99</v>
+      </c>
+      <c r="F152" t="s">
+        <v>1</v>
+      </c>
+      <c r="G152" t="b">
+        <v>0</v>
+      </c>
+      <c r="H152" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>100</v>
-      </c>
-      <c r="F152" t="s">
-        <v>1</v>
-      </c>
-      <c r="G152" t="b">
-        <v>0</v>
-      </c>
-      <c r="H152" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>101</v>
       </c>
       <c r="B153">
         <f t="shared" si="2"/>
@@ -4635,7 +4633,7 @@
         <v>18</v>
       </c>
       <c r="D153" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E153" t="s">
         <v>19</v>
@@ -4650,9 +4648,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B154">
         <f t="shared" si="2"/>
@@ -4677,9 +4675,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B155">
         <f t="shared" si="2"/>
@@ -4689,7 +4687,7 @@
         <v>13</v>
       </c>
       <c r="D155" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F155" t="s">
         <v>1</v>
@@ -4701,9 +4699,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B156">
         <f t="shared" si="2"/>
@@ -4713,21 +4711,21 @@
         <v>13</v>
       </c>
       <c r="D156" t="s">
+        <v>103</v>
+      </c>
+      <c r="F156" t="s">
+        <v>2</v>
+      </c>
+      <c r="G156" t="b">
+        <v>1</v>
+      </c>
+      <c r="H156" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>104</v>
-      </c>
-      <c r="F156" t="s">
-        <v>2</v>
-      </c>
-      <c r="G156" t="b">
-        <v>1</v>
-      </c>
-      <c r="H156" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>105</v>
       </c>
       <c r="B157">
         <f t="shared" si="2"/>
@@ -4737,7 +4735,7 @@
         <v>13</v>
       </c>
       <c r="D157" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F157" t="s">
         <v>2</v>
@@ -4749,9 +4747,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B158">
         <f t="shared" si="2"/>
@@ -4761,7 +4759,7 @@
         <v>18</v>
       </c>
       <c r="D158" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F158" t="s">
         <v>1</v>
@@ -4773,9 +4771,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B159">
         <f t="shared" si="2"/>
@@ -4785,7 +4783,7 @@
         <v>18</v>
       </c>
       <c r="D159" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E159" t="s">
         <v>19</v>
@@ -4800,9 +4798,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B160">
         <f t="shared" si="2"/>
@@ -4827,9 +4825,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B161">
         <f t="shared" si="2"/>
@@ -4839,7 +4837,7 @@
         <v>13</v>
       </c>
       <c r="D161" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F161" t="s">
         <v>1</v>
@@ -4851,9 +4849,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B162">
         <f t="shared" si="2"/>
@@ -4863,7 +4861,7 @@
         <v>13</v>
       </c>
       <c r="D162" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F162" t="s">
         <v>2</v>
@@ -4875,9 +4873,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B163">
         <f t="shared" si="2"/>
@@ -4887,7 +4885,7 @@
         <v>13</v>
       </c>
       <c r="D163" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F163" t="s">
         <v>2</v>
@@ -4899,9 +4897,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B164">
         <f t="shared" si="2"/>
@@ -4911,7 +4909,7 @@
         <v>18</v>
       </c>
       <c r="D164" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F164" t="s">
         <v>1</v>
@@ -4923,9 +4921,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B165">
         <f t="shared" si="2"/>
@@ -4935,7 +4933,7 @@
         <v>18</v>
       </c>
       <c r="D165" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E165" t="s">
         <v>19</v>
@@ -4950,9 +4948,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B166">
         <f t="shared" si="2"/>
@@ -4977,9 +4975,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B167">
         <f t="shared" si="2"/>
@@ -4989,7 +4987,7 @@
         <v>13</v>
       </c>
       <c r="D167" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F167" t="s">
         <v>1</v>
@@ -5001,9 +4999,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B168">
         <f t="shared" si="2"/>
@@ -5013,7 +5011,7 @@
         <v>13</v>
       </c>
       <c r="D168" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F168" t="s">
         <v>2</v>
@@ -5025,9 +5023,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B169">
         <f t="shared" si="2"/>
@@ -5037,21 +5035,21 @@
         <v>13</v>
       </c>
       <c r="D169" t="s">
+        <v>112</v>
+      </c>
+      <c r="F169" t="s">
+        <v>2</v>
+      </c>
+      <c r="G169" t="b">
+        <v>1</v>
+      </c>
+      <c r="H169" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
         <v>113</v>
-      </c>
-      <c r="F169" t="s">
-        <v>2</v>
-      </c>
-      <c r="G169" t="b">
-        <v>1</v>
-      </c>
-      <c r="H169" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>114</v>
       </c>
       <c r="B170">
         <f t="shared" si="2"/>
@@ -5061,7 +5059,7 @@
         <v>18</v>
       </c>
       <c r="D170" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F170" t="s">
         <v>1</v>
@@ -5073,9 +5071,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B171">
         <f t="shared" si="2"/>
@@ -5085,7 +5083,7 @@
         <v>18</v>
       </c>
       <c r="D171" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E171" t="s">
         <v>19</v>
@@ -5100,9 +5098,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B172">
         <f t="shared" si="2"/>
@@ -5127,9 +5125,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B173">
         <f t="shared" si="2"/>
@@ -5139,7 +5137,7 @@
         <v>13</v>
       </c>
       <c r="D173" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F173" t="s">
         <v>1</v>
@@ -5151,9 +5149,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B174">
         <f t="shared" si="2"/>
@@ -5163,7 +5161,7 @@
         <v>13</v>
       </c>
       <c r="D174" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F174" t="s">
         <v>2</v>
@@ -5175,9 +5173,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B175">
         <f t="shared" si="2"/>
@@ -5187,7 +5185,7 @@
         <v>13</v>
       </c>
       <c r="D175" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F175" t="s">
         <v>2</v>
@@ -5199,9 +5197,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B176">
         <f t="shared" si="2"/>
@@ -5211,7 +5209,7 @@
         <v>18</v>
       </c>
       <c r="D176" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F176" t="s">
         <v>1</v>
@@ -5223,9 +5221,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B177">
         <f t="shared" si="2"/>
@@ -5235,21 +5233,21 @@
         <v>18</v>
       </c>
       <c r="D177" t="s">
+        <v>117</v>
+      </c>
+      <c r="F177" t="s">
+        <v>1</v>
+      </c>
+      <c r="G177" t="b">
+        <v>0</v>
+      </c>
+      <c r="H177" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
         <v>118</v>
-      </c>
-      <c r="F177" t="s">
-        <v>1</v>
-      </c>
-      <c r="G177" t="b">
-        <v>0</v>
-      </c>
-      <c r="H177" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>119</v>
       </c>
       <c r="B178">
         <f t="shared" si="2"/>
@@ -5259,7 +5257,7 @@
         <v>18</v>
       </c>
       <c r="D178" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E178" t="s">
         <v>19</v>
@@ -5274,9 +5272,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B179">
         <f t="shared" si="2"/>
@@ -5301,9 +5299,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B180">
         <f t="shared" si="2"/>
@@ -5313,7 +5311,7 @@
         <v>13</v>
       </c>
       <c r="D180" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F180" t="s">
         <v>1</v>
@@ -5325,9 +5323,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B181">
         <f t="shared" si="2"/>
@@ -5337,7 +5335,7 @@
         <v>13</v>
       </c>
       <c r="D181" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F181" t="s">
         <v>2</v>
@@ -5349,9 +5347,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B182">
         <f t="shared" si="2"/>
@@ -5361,7 +5359,7 @@
         <v>13</v>
       </c>
       <c r="D182" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F182" t="s">
         <v>2</v>
@@ -5373,9 +5371,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B183">
         <f t="shared" si="2"/>
@@ -5385,7 +5383,7 @@
         <v>18</v>
       </c>
       <c r="D183" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F183" t="s">
         <v>1</v>
@@ -5397,9 +5395,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B184">
         <f t="shared" si="2"/>
@@ -5409,7 +5407,7 @@
         <v>18</v>
       </c>
       <c r="D184" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F184" t="s">
         <v>1</v>
@@ -5421,9 +5419,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B185">
         <f t="shared" si="2"/>
@@ -5433,7 +5431,7 @@
         <v>18</v>
       </c>
       <c r="D185" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F185" t="s">
         <v>1</v>
@@ -5445,9 +5443,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B186">
         <f t="shared" si="2"/>
@@ -5457,21 +5455,21 @@
         <v>18</v>
       </c>
       <c r="D186" t="s">
+        <v>122</v>
+      </c>
+      <c r="F186" t="s">
+        <v>1</v>
+      </c>
+      <c r="G186" t="b">
+        <v>0</v>
+      </c>
+      <c r="H186" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
         <v>123</v>
-      </c>
-      <c r="F186" t="s">
-        <v>1</v>
-      </c>
-      <c r="G186" t="b">
-        <v>0</v>
-      </c>
-      <c r="H186" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>124</v>
       </c>
       <c r="B187">
         <f t="shared" si="2"/>
@@ -5481,7 +5479,7 @@
         <v>18</v>
       </c>
       <c r="D187" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E187" t="s">
         <v>19</v>
@@ -5496,9 +5494,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B188">
         <f t="shared" si="2"/>
@@ -5523,9 +5521,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B189">
         <f t="shared" si="2"/>
@@ -5535,7 +5533,7 @@
         <v>13</v>
       </c>
       <c r="D189" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F189" t="s">
         <v>1</v>
@@ -5547,9 +5545,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B190">
         <f t="shared" si="2"/>
@@ -5559,7 +5557,7 @@
         <v>13</v>
       </c>
       <c r="D190" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F190" t="s">
         <v>2</v>
@@ -5571,9 +5569,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B191">
         <f t="shared" si="2"/>
@@ -5583,7 +5581,7 @@
         <v>13</v>
       </c>
       <c r="D191" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F191" t="s">
         <v>2</v>
@@ -5595,9 +5593,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B192">
         <f t="shared" si="2"/>
@@ -5607,7 +5605,7 @@
         <v>18</v>
       </c>
       <c r="D192" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F192" t="s">
         <v>1</v>
@@ -5619,9 +5617,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B193">
         <f t="shared" si="2"/>
@@ -5631,7 +5629,7 @@
         <v>18</v>
       </c>
       <c r="D193" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F193" t="s">
         <v>1</v>
@@ -5643,9 +5641,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B194">
         <f t="shared" si="2"/>
@@ -5655,7 +5653,7 @@
         <v>18</v>
       </c>
       <c r="D194" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F194" t="s">
         <v>1</v>
@@ -5667,9 +5665,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B195">
         <f t="shared" ref="B195:B225" si="3">IF(AND(A194=A195, C194=C195), B194+1, 1)</f>
@@ -5679,7 +5677,7 @@
         <v>18</v>
       </c>
       <c r="D195" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F195" t="s">
         <v>1</v>
@@ -5691,9 +5689,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B196">
         <f t="shared" si="3"/>
@@ -5703,7 +5701,7 @@
         <v>18</v>
       </c>
       <c r="D196" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E196" t="s">
         <v>19</v>
@@ -5718,9 +5716,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B197">
         <f t="shared" si="3"/>
@@ -5745,9 +5743,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B198">
         <f t="shared" si="3"/>
@@ -5757,7 +5755,7 @@
         <v>13</v>
       </c>
       <c r="D198" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F198" t="s">
         <v>1</v>
@@ -5769,9 +5767,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B199">
         <f t="shared" si="3"/>
@@ -5781,21 +5779,21 @@
         <v>13</v>
       </c>
       <c r="D199" t="s">
+        <v>128</v>
+      </c>
+      <c r="F199" t="s">
+        <v>2</v>
+      </c>
+      <c r="G199" t="b">
+        <v>1</v>
+      </c>
+      <c r="H199" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
         <v>129</v>
-      </c>
-      <c r="F199" t="s">
-        <v>2</v>
-      </c>
-      <c r="G199" t="b">
-        <v>1</v>
-      </c>
-      <c r="H199" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
-        <v>130</v>
       </c>
       <c r="B200">
         <f t="shared" si="3"/>
@@ -5805,7 +5803,7 @@
         <v>13</v>
       </c>
       <c r="D200" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F200" t="s">
         <v>2</v>
@@ -5817,9 +5815,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B201">
         <f t="shared" si="3"/>
@@ -5829,7 +5827,7 @@
         <v>18</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F201" t="s">
         <v>1</v>
@@ -5841,9 +5839,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B202">
         <f t="shared" si="3"/>
@@ -5853,7 +5851,7 @@
         <v>18</v>
       </c>
       <c r="D202" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E202" t="s">
         <v>19</v>
@@ -5868,9 +5866,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B203">
         <f t="shared" si="3"/>
@@ -5895,9 +5893,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B204">
         <f t="shared" si="3"/>
@@ -5907,7 +5905,7 @@
         <v>13</v>
       </c>
       <c r="D204" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F204" t="s">
         <v>1</v>
@@ -5919,9 +5917,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B205">
         <f t="shared" si="3"/>
@@ -5931,7 +5929,7 @@
         <v>13</v>
       </c>
       <c r="D205" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F205" t="s">
         <v>2</v>
@@ -5943,9 +5941,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B206">
         <f t="shared" si="3"/>
@@ -5955,21 +5953,21 @@
         <v>13</v>
       </c>
       <c r="D206" t="s">
+        <v>133</v>
+      </c>
+      <c r="F206" t="s">
+        <v>2</v>
+      </c>
+      <c r="G206" t="b">
+        <v>1</v>
+      </c>
+      <c r="H206" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
         <v>134</v>
-      </c>
-      <c r="F206" t="s">
-        <v>2</v>
-      </c>
-      <c r="G206" t="b">
-        <v>1</v>
-      </c>
-      <c r="H206" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>135</v>
       </c>
       <c r="B207">
         <f t="shared" si="3"/>
@@ -5979,7 +5977,7 @@
         <v>18</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F207" t="s">
         <v>1</v>
@@ -5991,9 +5989,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B208">
         <f t="shared" si="3"/>
@@ -6003,7 +6001,7 @@
         <v>18</v>
       </c>
       <c r="D208" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E208" t="s">
         <v>19</v>
@@ -6018,9 +6016,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B209">
         <f t="shared" si="3"/>
@@ -6045,9 +6043,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B210">
         <f t="shared" si="3"/>
@@ -6057,7 +6055,7 @@
         <v>13</v>
       </c>
       <c r="D210" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F210" t="s">
         <v>1</v>
@@ -6069,9 +6067,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B211">
         <f t="shared" si="3"/>
@@ -6081,7 +6079,7 @@
         <v>13</v>
       </c>
       <c r="D211" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F211" t="s">
         <v>2</v>
@@ -6093,9 +6091,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B212">
         <f t="shared" si="3"/>
@@ -6105,7 +6103,7 @@
         <v>13</v>
       </c>
       <c r="D212" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F212" t="s">
         <v>2</v>
@@ -6117,9 +6115,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B213">
         <f t="shared" si="3"/>
@@ -6129,21 +6127,21 @@
         <v>18</v>
       </c>
       <c r="D213" t="s">
+        <v>137</v>
+      </c>
+      <c r="F213" t="s">
+        <v>1</v>
+      </c>
+      <c r="G213" t="b">
+        <v>0</v>
+      </c>
+      <c r="H213" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
         <v>138</v>
-      </c>
-      <c r="F213" t="s">
-        <v>1</v>
-      </c>
-      <c r="G213" t="b">
-        <v>0</v>
-      </c>
-      <c r="H213" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
-        <v>139</v>
       </c>
       <c r="B214">
         <f t="shared" si="3"/>
@@ -6153,7 +6151,7 @@
         <v>18</v>
       </c>
       <c r="D214" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E214" t="s">
         <v>19</v>
@@ -6168,9 +6166,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B215">
         <f t="shared" si="3"/>
@@ -6195,9 +6193,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B216">
         <f t="shared" si="3"/>
@@ -6207,7 +6205,7 @@
         <v>13</v>
       </c>
       <c r="D216" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F216" t="s">
         <v>1</v>
@@ -6219,9 +6217,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B217">
         <f t="shared" si="3"/>
@@ -6231,7 +6229,7 @@
         <v>13</v>
       </c>
       <c r="D217" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F217" t="s">
         <v>2</v>
@@ -6243,9 +6241,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B218">
         <f t="shared" si="3"/>
@@ -6255,21 +6253,21 @@
         <v>13</v>
       </c>
       <c r="D218" t="s">
+        <v>140</v>
+      </c>
+      <c r="F218" t="s">
+        <v>2</v>
+      </c>
+      <c r="G218" t="b">
+        <v>1</v>
+      </c>
+      <c r="H218" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
         <v>141</v>
-      </c>
-      <c r="F218" t="s">
-        <v>2</v>
-      </c>
-      <c r="G218" t="b">
-        <v>1</v>
-      </c>
-      <c r="H218" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
-        <v>142</v>
       </c>
       <c r="B219">
         <f t="shared" si="3"/>
@@ -6279,7 +6277,7 @@
         <v>18</v>
       </c>
       <c r="D219" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E219" t="s">
         <v>19</v>
@@ -6294,9 +6292,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B220">
         <f t="shared" si="3"/>
@@ -6321,9 +6319,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B221">
         <f t="shared" si="3"/>
@@ -6333,7 +6331,7 @@
         <v>13</v>
       </c>
       <c r="D221" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F221" t="s">
         <v>1</v>
@@ -6345,9 +6343,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B222">
         <f t="shared" si="3"/>
@@ -6357,7 +6355,7 @@
         <v>13</v>
       </c>
       <c r="D222" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F222" t="s">
         <v>2</v>
@@ -6369,9 +6367,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B223">
         <f t="shared" si="3"/>
@@ -6381,7 +6379,7 @@
         <v>13</v>
       </c>
       <c r="D223" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F223" t="s">
         <v>2</v>
@@ -6393,9 +6391,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B224">
         <f t="shared" si="3"/>
@@ -6405,21 +6403,21 @@
         <v>18</v>
       </c>
       <c r="D224" t="s">
+        <v>144</v>
+      </c>
+      <c r="F224" t="s">
+        <v>1</v>
+      </c>
+      <c r="G224" t="b">
+        <v>0</v>
+      </c>
+      <c r="H224" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
         <v>145</v>
-      </c>
-      <c r="F224" t="s">
-        <v>1</v>
-      </c>
-      <c r="G224" t="b">
-        <v>0</v>
-      </c>
-      <c r="H224" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
-        <v>146</v>
       </c>
       <c r="B225">
         <f t="shared" si="3"/>
@@ -6429,7 +6427,7 @@
         <v>18</v>
       </c>
       <c r="D225" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E225" t="s">
         <v>19</v>
@@ -6445,7 +6443,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I225" xr:uid="{D7EA4A85-694E-4AFC-88A1-1F9A25E65D09}"/>
+  <autoFilter ref="A1:I225" xr:uid="{D7EA4A85-694E-4AFC-88A1-1F9A25E65D09}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="14-3.01"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>